<commit_message>
Set up .gitattributes to track xls; added "hello world!" to SES quotes
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10200" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10201" uniqueCount="1123">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -613,7 +613,7 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
 How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
 Haven't seen how income was meausred. 
 </t>
@@ -697,7 +697,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -784,7 +784,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -944,7 +944,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1022,7 +1022,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1044,7 +1044,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1606,7 +1606,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x0001_f_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x0002_0,Z_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1658,11 +1658,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x0001_ 10.611, N _x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x0001_ 10.167, n _x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x0001_ 8.75, n _x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1739,26 +1739,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1875,7 +1875,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1884,12 +1884,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1914,7 +1914,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1949,9 +1949,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1984,7 +1984,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2040,8 +2040,8 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2156,7 +2156,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2215,7 +2215,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2226,7 +2226,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2272,7 +2272,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2372,7 +2372,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2520,7 +2520,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2579,7 +2579,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2621,7 +2621,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2706,7 +2706,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3089,7 +3089,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3159,19 +3159,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3299,7 +3299,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3443,7 +3443,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x0006_Mcommunity_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x0002_15.55,p_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3613,7 +3613,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3757,7 +3757,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3826,12 +3826,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3854,7 +3854,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3894,13 +3894,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3955,14 +3955,14 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4015,7 +4015,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4043,6 +4043,9 @@
   </si>
   <si>
     <t xml:space="preserve">Développement langagier et cognitif de l'enfant durant les trois premières années en relation avec la durée des vocalisations maternelles et les jouets présents dans l'environment: Étude longitudinale auprès de populations á risque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello world!</t>
   </si>
 </sst>
 </file>
@@ -16564,11 +16567,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16712,6 +16715,9 @@
       </c>
       <c r="H2" s="0" t="s">
         <v>40</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>1122</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Line edit to code sheet
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -16571,7 +16571,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16716,9 +16716,6 @@
       <c r="H2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>1122</v>
-      </c>
       <c r="K2" s="0" t="s">
         <v>41</v>
       </c>
@@ -16750,6 +16747,9 @@
       </c>
       <c r="H3" s="0" t="s">
         <v>40</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>1122</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Halfway through sesMainEffect column
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10201" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10193" uniqueCount="1123">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -4045,7 +4045,7 @@
     <t xml:space="preserve">Développement langagier et cognitif de l'enfant durant les trois premières années en relation avec la durée des vocalisations maternelles et les jouets présents dans l'environment: Étude longitudinale auprès de populations á risque</t>
   </si>
   <si>
-    <t xml:space="preserve">hello world!</t>
+    <t xml:space="preserve">Did not study SES</t>
   </si>
 </sst>
 </file>
@@ -4087,7 +4087,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4098,6 +4098,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
         <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -4135,7 +4141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4157,6 +4163,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4252,11 +4266,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E82" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F39" activeCellId="0" sqref="F39"/>
+      <selection pane="bottomLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="D106" activeCellId="0" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16567,11 +16581,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="J107" activeCellId="0" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16748,9 +16762,6 @@
       <c r="H3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>1122</v>
-      </c>
       <c r="L3" s="0" t="n">
         <v>6</v>
       </c>
@@ -17611,7 +17622,7 @@
         <v>41</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>41</v>
@@ -17661,10 +17672,10 @@
         <v>41</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K33" s="0" t="s">
         <v>165</v>
@@ -17708,7 +17719,7 @@
         <v>41</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>40</v>
@@ -17802,7 +17813,7 @@
         <v>41</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>40</v>
@@ -17849,10 +17860,7 @@
         <v>41</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>41</v>
@@ -17887,7 +17895,7 @@
         <v>41</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L38" s="0" t="n">
         <v>323</v>
@@ -17969,7 +17977,7 @@
         <v>41</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>41</v>
@@ -18019,7 +18027,7 @@
         <v>41</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>40</v>
@@ -18066,7 +18074,7 @@
         <v>41</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J42" s="0" t="s">
         <v>41</v>
@@ -18116,7 +18124,7 @@
         <v>41</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J43" s="0" t="s">
         <v>40</v>
@@ -18163,7 +18171,7 @@
         <v>41</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>40</v>
@@ -18269,7 +18277,7 @@
         <v>41</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>40</v>
@@ -18322,7 +18330,7 @@
         <v>41</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J47" s="0" t="s">
         <v>40</v>
@@ -18369,7 +18377,7 @@
         <v>41</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J48" s="0" t="s">
         <v>41</v>
@@ -18419,7 +18427,7 @@
         <v>41</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J49" s="0" t="s">
         <v>40</v>
@@ -18516,7 +18524,7 @@
         <v>41</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>41</v>
@@ -18610,7 +18618,7 @@
         <v>41</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>41</v>
@@ -18657,7 +18665,7 @@
         <v>41</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J54" s="0" t="s">
         <v>40</v>
@@ -18757,7 +18765,7 @@
         <v>41</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L56" s="0" t="n">
         <v>397</v>
@@ -18839,7 +18847,7 @@
         <v>41</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J58" s="0" t="s">
         <v>40</v>
@@ -18889,7 +18897,7 @@
         <v>41</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J59" s="0" t="s">
         <v>41</v>
@@ -18939,7 +18947,7 @@
         <v>41</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J60" s="0" t="s">
         <v>40</v>
@@ -19048,7 +19056,7 @@
         <v>41</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>40</v>
@@ -19139,10 +19147,10 @@
         <v>41</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>165</v>
@@ -19186,7 +19194,7 @@
         <v>41</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J65" s="0" t="s">
         <v>41</v>
@@ -19233,7 +19241,7 @@
         <v>41</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J66" s="0" t="s">
         <v>41</v>
@@ -19283,7 +19291,7 @@
         <v>41</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J67" s="0" t="s">
         <v>41</v>
@@ -19383,7 +19391,7 @@
         <v>41</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J69" s="0" t="s">
         <v>40</v>
@@ -19433,7 +19441,7 @@
         <v>41</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J70" s="0" t="s">
         <v>40</v>
@@ -19483,7 +19491,7 @@
         <v>41</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J71" s="0" t="s">
         <v>41</v>
@@ -19627,10 +19635,7 @@
         <v>41</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K74" s="0" t="s">
         <v>41</v>
@@ -19677,10 +19682,7 @@
         <v>41</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J75" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K75" s="0" t="s">
         <v>41</v>
@@ -19715,7 +19717,7 @@
         <v>41</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L76" s="0" t="n">
         <v>21</v>
@@ -19779,7 +19781,7 @@
         <v>41</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J78" s="0" t="s">
         <v>41</v>
@@ -19826,7 +19828,7 @@
         <v>41</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J79" s="0" t="s">
         <v>41</v>
@@ -19873,7 +19875,7 @@
         <v>41</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>41</v>
@@ -19967,7 +19969,7 @@
         <v>41</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>41</v>
@@ -20014,10 +20016,7 @@
         <v>41</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>41</v>
@@ -20102,7 +20101,7 @@
         <v>41</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L85" s="4" t="n">
         <v>59</v>
@@ -20134,7 +20133,7 @@
         <v>41</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J86" s="0" t="s">
         <v>40</v>
@@ -20184,7 +20183,7 @@
         <v>41</v>
       </c>
       <c r="I87" s="0" t="s">
-        <v>380</v>
+        <v>444</v>
       </c>
       <c r="J87" s="0" t="s">
         <v>40</v>
@@ -20231,10 +20230,7 @@
         <v>41</v>
       </c>
       <c r="I88" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J88" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K88" s="0" t="s">
         <v>41</v>
@@ -20281,7 +20277,7 @@
         <v>41</v>
       </c>
       <c r="I89" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J89" s="0" t="s">
         <v>40</v>
@@ -20331,7 +20327,7 @@
         <v>41</v>
       </c>
       <c r="I90" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J90" s="0" t="s">
         <v>41</v>
@@ -20381,10 +20377,7 @@
         <v>41</v>
       </c>
       <c r="I91" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J91" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K91" s="0" t="s">
         <v>41</v>
@@ -20422,7 +20415,7 @@
         <v>41</v>
       </c>
       <c r="I92" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J92" s="0" t="s">
         <v>41</v>
@@ -20469,7 +20462,7 @@
         <v>41</v>
       </c>
       <c r="I93" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J93" s="0" t="s">
         <v>40</v>
@@ -20516,10 +20509,7 @@
         <v>41</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J94" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="K94" s="0" t="s">
         <v>41</v>
@@ -20554,7 +20544,7 @@
         <v>41</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J95" s="0" t="s">
         <v>41</v>
@@ -20648,7 +20638,7 @@
         <v>41</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J97" s="0" t="s">
         <v>40</v>
@@ -20695,7 +20685,7 @@
         <v>41</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J98" s="0" t="s">
         <v>41</v>
@@ -20745,7 +20735,7 @@
         <v>41</v>
       </c>
       <c r="I99" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J99" s="4" t="s">
         <v>40</v>
@@ -20795,7 +20785,7 @@
         <v>41</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="J100" s="4" t="s">
         <v>41</v>
@@ -20842,7 +20832,7 @@
         <v>41</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J101" s="0" t="s">
         <v>40</v>
@@ -20939,7 +20929,7 @@
         <v>41</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J103" s="0" t="s">
         <v>40</v>
@@ -20986,7 +20976,7 @@
         <v>41</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J104" s="0" t="s">
         <v>40</v>
@@ -21036,7 +21026,7 @@
         <v>41</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J105" s="0" t="s">
         <v>40</v>
@@ -21060,53 +21050,53 @@
         <v>460</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+    <row r="106" s="6" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C106" s="0" t="n">
+      <c r="C106" s="6" t="n">
         <v>2005</v>
       </c>
-      <c r="D106" s="0" t="s">
+      <c r="D106" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="E106" s="0" t="s">
+      <c r="E106" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F106" s="0" t="s">
+      <c r="F106" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="G106" s="0" t="s">
+      <c r="G106" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H106" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I106" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J106" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K106" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L106" s="0" t="n">
+      <c r="H106" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J106" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K106" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L106" s="6" t="n">
         <v>172</v>
       </c>
-      <c r="M106" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N106" s="0" t="s">
+      <c r="M106" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N106" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="O106" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH106" s="3" t="s">
+      <c r="O106" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH106" s="7" t="s">
         <v>465</v>
       </c>
     </row>
@@ -21136,7 +21126,7 @@
         <v>41</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J107" s="0" t="s">
         <v>40</v>
@@ -21239,7 +21229,7 @@
         <v>41</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J109" s="0" t="s">
         <v>41</v>
@@ -21277,7 +21267,7 @@
         <v>41</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J110" s="0" t="s">
         <v>41</v>
@@ -21327,7 +21317,7 @@
         <v>41</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J111" s="0" t="s">
         <v>40</v>
@@ -21377,7 +21367,7 @@
         <v>41</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J112" s="4" t="s">
         <v>40</v>
@@ -21474,7 +21464,7 @@
         <v>41</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J114" s="4" t="s">
         <v>40</v>
@@ -21524,7 +21514,7 @@
         <v>41</v>
       </c>
       <c r="I115" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J115" s="0" t="s">
         <v>41</v>
@@ -21574,7 +21564,7 @@
         <v>41</v>
       </c>
       <c r="I116" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J116" s="0" t="s">
         <v>41</v>
@@ -21624,7 +21614,7 @@
         <v>41</v>
       </c>
       <c r="I117" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L117" s="0" t="n">
         <v>12</v>
@@ -21656,7 +21646,7 @@
         <v>41</v>
       </c>
       <c r="I118" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J118" s="0" t="s">
         <v>40</v>
@@ -21703,7 +21693,7 @@
         <v>41</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J119" s="4" t="s">
         <v>41</v>
@@ -21803,7 +21793,7 @@
         <v>41</v>
       </c>
       <c r="I121" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J121" s="4" t="s">
         <v>41</v>
@@ -21850,7 +21840,7 @@
         <v>41</v>
       </c>
       <c r="I122" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J122" s="4" t="s">
         <v>40</v>
@@ -21947,7 +21937,7 @@
         <v>41</v>
       </c>
       <c r="I124" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J124" s="4" t="s">
         <v>165</v>
@@ -21994,7 +21984,7 @@
         <v>41</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J125" s="0" t="s">
         <v>41</v>
@@ -22091,7 +22081,7 @@
         <v>41</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J127" s="0" t="s">
         <v>41</v>
@@ -22129,7 +22119,7 @@
         <v>41</v>
       </c>
       <c r="I128" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J128" s="4" t="s">
         <v>40</v>
@@ -22179,7 +22169,7 @@
         <v>41</v>
       </c>
       <c r="I129" s="4" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="J129" s="4" t="s">
         <v>40</v>
@@ -22276,7 +22266,7 @@
         <v>41</v>
       </c>
       <c r="I131" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J131" s="0" t="s">
         <v>40</v>
@@ -22326,7 +22316,7 @@
         <v>41</v>
       </c>
       <c r="I132" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="J132" s="0" t="s">
         <v>40</v>
@@ -22373,7 +22363,7 @@
         <v>41</v>
       </c>
       <c r="I133" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J133" s="0" t="s">
         <v>40</v>
@@ -22420,7 +22410,7 @@
         <v>41</v>
       </c>
       <c r="I134" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J134" s="0" t="s">
         <v>41</v>
@@ -22470,7 +22460,7 @@
         <v>41</v>
       </c>
       <c r="I135" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J135" s="0" t="s">
         <v>40</v>
@@ -22517,7 +22507,7 @@
         <v>41</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J136" s="4" t="s">
         <v>40</v>
@@ -22611,7 +22601,7 @@
         <v>41</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J138" s="4" t="s">
         <v>165</v>
@@ -22705,7 +22695,7 @@
         <v>41</v>
       </c>
       <c r="I140" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J140" s="0" t="s">
         <v>41</v>
@@ -22752,7 +22742,7 @@
         <v>41</v>
       </c>
       <c r="I141" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J141" s="0" t="s">
         <v>41</v>
@@ -22802,7 +22792,7 @@
         <v>41</v>
       </c>
       <c r="I142" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J142" s="0" t="s">
         <v>41</v>
@@ -22849,7 +22839,7 @@
         <v>41</v>
       </c>
       <c r="I143" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J143" s="0" t="s">
         <v>40</v>
@@ -22896,7 +22886,7 @@
         <v>41</v>
       </c>
       <c r="I144" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>41</v>
@@ -22993,7 +22983,7 @@
         <v>41</v>
       </c>
       <c r="I146" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J146" s="0" t="s">
         <v>40</v>
@@ -23093,7 +23083,7 @@
         <v>41</v>
       </c>
       <c r="I148" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J148" s="0" t="s">
         <v>41</v>
@@ -23199,7 +23189,7 @@
         <v>41</v>
       </c>
       <c r="I150" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J150" s="4" t="s">
         <v>40</v>
@@ -23293,7 +23283,7 @@
         <v>41</v>
       </c>
       <c r="I152" s="4" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J152" s="4" t="s">
         <v>40</v>
@@ -23419,7 +23409,7 @@
         <v>41</v>
       </c>
       <c r="I155" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J155" s="0" t="s">
         <v>41</v>
@@ -23469,7 +23459,7 @@
         <v>41</v>
       </c>
       <c r="I156" s="4" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J156" s="4" t="s">
         <v>41</v>
@@ -23504,7 +23494,7 @@
         <v>41</v>
       </c>
       <c r="I157" s="4" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J157" s="4" t="s">
         <v>41</v>
@@ -23539,7 +23529,7 @@
         <v>41</v>
       </c>
       <c r="I158" s="4" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J158" s="4" t="s">
         <v>41</v>
@@ -23574,7 +23564,7 @@
         <v>41</v>
       </c>
       <c r="I159" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J159" s="0" t="s">
         <v>40</v>
@@ -23621,7 +23611,7 @@
         <v>41</v>
       </c>
       <c r="I160" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L160" s="0" t="n">
         <v>19</v>
@@ -23653,7 +23643,7 @@
         <v>41</v>
       </c>
       <c r="I161" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J161" s="0" t="s">
         <v>40</v>
@@ -23703,7 +23693,7 @@
         <v>41</v>
       </c>
       <c r="I162" s="0" t="s">
-        <v>380</v>
+        <v>444</v>
       </c>
       <c r="J162" s="0" t="s">
         <v>41</v>
@@ -23800,7 +23790,7 @@
         <v>41</v>
       </c>
       <c r="I164" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J164" s="0" t="s">
         <v>679</v>
@@ -23897,7 +23887,7 @@
         <v>41</v>
       </c>
       <c r="I166" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J166" s="0" t="s">
         <v>40</v>
@@ -23944,7 +23934,7 @@
         <v>41</v>
       </c>
       <c r="I167" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J167" s="0" t="s">
         <v>40</v>
@@ -24009,7 +23999,7 @@
         <v>41</v>
       </c>
       <c r="I168" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>40</v>
@@ -24109,7 +24099,7 @@
         <v>41</v>
       </c>
       <c r="I170" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J170" s="4" t="s">
         <v>40</v>
@@ -24239,7 +24229,7 @@
         <v>41</v>
       </c>
       <c r="I172" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J172" s="4" t="s">
         <v>40</v>
@@ -24304,7 +24294,7 @@
         <v>41</v>
       </c>
       <c r="I173" s="4" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J173" s="4" t="s">
         <v>41</v>
@@ -24486,7 +24476,7 @@
         <v>41</v>
       </c>
       <c r="I177" s="4" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J177" s="4" t="s">
         <v>41</v>
@@ -24553,7 +24543,7 @@
         <v>41</v>
       </c>
       <c r="I179" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J179" s="4" t="s">
         <v>40</v>
@@ -24647,7 +24637,7 @@
         <v>41</v>
       </c>
       <c r="I181" s="4" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="J181" s="4" t="s">
         <v>165</v>
@@ -24744,7 +24734,7 @@
         <v>41</v>
       </c>
       <c r="I183" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J183" s="0" t="s">
         <v>40</v>
@@ -24791,7 +24781,7 @@
         <v>41</v>
       </c>
       <c r="I184" s="0" t="s">
-        <v>743</v>
+        <v>1122</v>
       </c>
       <c r="L184" s="0" t="n">
         <v>82</v>
@@ -24876,7 +24866,7 @@
         <v>41</v>
       </c>
       <c r="I186" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L186" s="0" t="n">
         <v>0</v>
@@ -24911,7 +24901,7 @@
         <v>41</v>
       </c>
       <c r="I187" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J187" s="0" t="s">
         <v>41</v>
@@ -25064,7 +25054,7 @@
         <v>41</v>
       </c>
       <c r="I190" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J190" s="0" t="s">
         <v>41</v>
@@ -25114,7 +25104,7 @@
         <v>41</v>
       </c>
       <c r="I191" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J191" s="4" t="s">
         <v>40</v>
@@ -25208,7 +25198,7 @@
         <v>41</v>
       </c>
       <c r="I193" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J193" s="4" t="s">
         <v>40</v>
@@ -25352,7 +25342,7 @@
         <v>41</v>
       </c>
       <c r="I196" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J196" s="0" t="s">
         <v>41</v>
@@ -25402,7 +25392,7 @@
         <v>41</v>
       </c>
       <c r="I197" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J197" s="0" t="s">
         <v>41</v>
@@ -25452,7 +25442,7 @@
         <v>41</v>
       </c>
       <c r="I198" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J198" s="0" t="s">
         <v>40</v>
@@ -25582,7 +25572,7 @@
         <v>41</v>
       </c>
       <c r="I200" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J200" s="0" t="s">
         <v>41</v>
@@ -25717,7 +25707,7 @@
         <v>41</v>
       </c>
       <c r="I203" s="4" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J203" s="4" t="s">
         <v>41</v>
@@ -25758,7 +25748,7 @@
         <v>41</v>
       </c>
       <c r="I204" s="4" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L204" s="4" t="n">
         <v>3</v>
@@ -25790,7 +25780,7 @@
         <v>41</v>
       </c>
       <c r="I205" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J205" s="0" t="s">
         <v>40</v>
@@ -25887,7 +25877,7 @@
         <v>41</v>
       </c>
       <c r="I207" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J207" s="0" t="s">
         <v>41</v>
@@ -25937,7 +25927,7 @@
         <v>41</v>
       </c>
       <c r="I208" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L208" s="0" t="n">
         <v>73</v>
@@ -25969,7 +25959,7 @@
         <v>41</v>
       </c>
       <c r="I209" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J209" s="4" t="s">
         <v>40</v>
@@ -26055,7 +26045,7 @@
         <v>41</v>
       </c>
       <c r="I210" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J210" s="4" t="s">
         <v>40</v>
@@ -26158,7 +26148,7 @@
         <v>41</v>
       </c>
       <c r="I212" s="4" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J212" s="4" t="s">
         <v>40</v>
@@ -26205,7 +26195,7 @@
         <v>41</v>
       </c>
       <c r="I213" s="0" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J213" s="0" t="s">
         <v>41</v>
@@ -26255,7 +26245,7 @@
         <v>41</v>
       </c>
       <c r="I214" s="0" t="s">
-        <v>178</v>
+        <v>1122</v>
       </c>
       <c r="J214" s="0" t="s">
         <v>165</v>
@@ -26302,7 +26292,7 @@
         <v>41</v>
       </c>
       <c r="I215" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J215" s="4" t="s">
         <v>41</v>
@@ -26414,7 +26404,7 @@
         <v>41</v>
       </c>
       <c r="I217" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J217" s="4" t="s">
         <v>41</v>
@@ -26467,7 +26457,7 @@
         <v>41</v>
       </c>
       <c r="I218" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J218" s="4" t="s">
         <v>41</v>
@@ -26573,7 +26563,7 @@
         <v>41</v>
       </c>
       <c r="I220" s="4" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="J220" s="4" t="s">
         <v>41</v>
@@ -26685,7 +26675,7 @@
         <v>41</v>
       </c>
       <c r="I222" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J222" s="0" t="s">
         <v>41</v>
@@ -26732,7 +26722,7 @@
         <v>41</v>
       </c>
       <c r="I223" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J223" s="4" t="s">
         <v>40</v>
@@ -26897,7 +26887,7 @@
         <v>41</v>
       </c>
       <c r="I226" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L226" s="0" t="n">
         <v>0</v>
@@ -26982,7 +26972,7 @@
         <v>41</v>
       </c>
       <c r="I228" s="0" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="J228" s="0" t="s">
         <v>165</v>
@@ -27029,7 +27019,7 @@
         <v>41</v>
       </c>
       <c r="I229" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J229" s="0" t="s">
         <v>40</v>
@@ -27094,7 +27084,7 @@
         <v>41</v>
       </c>
       <c r="I230" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J230" s="0" t="s">
         <v>40</v>
@@ -27144,7 +27134,7 @@
         <v>41</v>
       </c>
       <c r="I231" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J231" s="0" t="s">
         <v>40</v>
@@ -27191,7 +27181,7 @@
         <v>41</v>
       </c>
       <c r="I232" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J232" s="0" t="s">
         <v>40</v>
@@ -27253,7 +27243,7 @@
         <v>41</v>
       </c>
       <c r="I233" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J233" s="0" t="s">
         <v>41</v>
@@ -27303,7 +27293,7 @@
         <v>41</v>
       </c>
       <c r="I234" s="0" t="s">
-        <v>41</v>
+        <v>1122</v>
       </c>
       <c r="J234" s="0" t="s">
         <v>41</v>
@@ -27362,7 +27352,7 @@
         <v>41</v>
       </c>
       <c r="I235" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J235" s="0" t="s">
         <v>41</v>
@@ -27409,7 +27399,7 @@
         <v>41</v>
       </c>
       <c r="I236" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J236" s="0" t="s">
         <v>40</v>
@@ -27468,7 +27458,7 @@
         <v>41</v>
       </c>
       <c r="I237" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J237" s="0" t="s">
         <v>40</v>
@@ -27530,7 +27520,7 @@
         <v>41</v>
       </c>
       <c r="I238" s="0" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="J238" s="0" t="s">
         <v>40</v>
@@ -27680,7 +27670,7 @@
         <v>41</v>
       </c>
       <c r="I241" s="0" t="s">
-        <v>743</v>
+        <v>1122</v>
       </c>
       <c r="L241" s="0" t="n">
         <v>167</v>
@@ -27715,7 +27705,7 @@
         <v>41</v>
       </c>
       <c r="I242" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J242" s="0" t="s">
         <v>40</v>
@@ -27815,7 +27805,7 @@
         <v>41</v>
       </c>
       <c r="I244" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J244" s="4" t="s">
         <v>40</v>
@@ -27951,7 +27941,7 @@
         <v>41</v>
       </c>
       <c r="I246" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J246" s="4" t="s">
         <v>40</v>
@@ -28016,7 +28006,7 @@
         <v>41</v>
       </c>
       <c r="I247" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J247" s="0" t="s">
         <v>40</v>
@@ -28090,7 +28080,7 @@
         <v>41</v>
       </c>
       <c r="I248" s="0" t="s">
-        <v>187</v>
+        <v>1122</v>
       </c>
       <c r="L248" s="0" t="n">
         <v>14</v>
@@ -28125,7 +28115,7 @@
         <v>41</v>
       </c>
       <c r="I249" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J249" s="0" t="s">
         <v>40</v>
@@ -28172,7 +28162,7 @@
         <v>41</v>
       </c>
       <c r="I250" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J250" s="0" t="s">
         <v>40</v>
@@ -28369,7 +28359,7 @@
         <v>41</v>
       </c>
       <c r="I254" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J254" s="0" t="s">
         <v>40</v>
@@ -28428,7 +28418,7 @@
         <v>41</v>
       </c>
       <c r="I255" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J255" s="0" t="s">
         <v>40</v>
@@ -28502,7 +28492,7 @@
         <v>41</v>
       </c>
       <c r="I256" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J256" s="0" t="s">
         <v>40</v>
@@ -28552,7 +28542,7 @@
         <v>41</v>
       </c>
       <c r="I257" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J257" s="0" t="s">
         <v>40</v>
@@ -28661,7 +28651,7 @@
         <v>41</v>
       </c>
       <c r="I259" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J259" s="0" t="s">
         <v>40</v>
@@ -28711,7 +28701,7 @@
         <v>41</v>
       </c>
       <c r="I260" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J260" s="0" t="s">
         <v>41</v>
@@ -28770,7 +28760,7 @@
         <v>41</v>
       </c>
       <c r="I261" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="J261" s="0" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Finished cleaning codes for not-quote variables
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10193" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10168" uniqueCount="1123">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -613,7 +613,7 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
 How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
 Haven't seen how income was meausred. 
 </t>
@@ -697,7 +697,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -784,7 +784,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -944,7 +944,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1022,7 +1022,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1044,7 +1044,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1606,7 +1606,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1658,11 +1658,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1739,26 +1739,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1875,7 +1875,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1884,12 +1884,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1914,7 +1914,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1949,9 +1949,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1984,7 +1984,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2040,8 +2040,8 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2156,7 +2156,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2215,7 +2215,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2226,7 +2226,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2272,7 +2272,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2372,7 +2372,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2520,7 +2520,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2579,7 +2579,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2621,7 +2621,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2706,7 +2706,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3089,7 +3089,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3159,19 +3159,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3299,7 +3299,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3443,7 +3443,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3613,7 +3613,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3757,7 +3757,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3826,12 +3826,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3854,7 +3854,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3894,13 +3894,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3955,14 +3955,14 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4015,7 +4015,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4266,11 +4266,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E104" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
-      <selection pane="bottomRight" activeCell="D106" activeCellId="0" sqref="D106"/>
+      <selection pane="bottomLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+      <selection pane="bottomRight" activeCell="I125" activeCellId="0" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16581,11 +16581,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E246" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
-      <selection pane="bottomRight" activeCell="J107" activeCellId="0" sqref="J107"/>
+      <selection pane="bottomLeft" activeCell="A246" activeCellId="0" sqref="A246"/>
+      <selection pane="bottomRight" activeCell="K262" activeCellId="0" sqref="K262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17678,7 +17678,7 @@
         <v>40</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L33" s="0" t="n">
         <v>30</v>
@@ -17862,9 +17862,6 @@
       <c r="I37" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="K37" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L37" s="0" t="n">
         <v>73</v>
       </c>
@@ -19153,7 +19150,7 @@
         <v>40</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L64" s="4" t="n">
         <v>6</v>
@@ -19637,9 +19634,6 @@
       <c r="I74" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="K74" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L74" s="0" t="n">
         <v>0</v>
       </c>
@@ -19684,9 +19678,6 @@
       <c r="I75" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="K75" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L75" s="0" t="n">
         <v>15</v>
       </c>
@@ -19834,7 +19825,7 @@
         <v>41</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L79" s="0" t="n">
         <v>41</v>
@@ -20018,9 +20009,6 @@
       <c r="I83" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="K83" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="L83" s="4" t="n">
         <v>59</v>
       </c>
@@ -20204,50 +20192,53 @@
         <v>382</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" s="6" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="C88" s="0" t="n">
+      <c r="C88" s="6" t="n">
         <v>2015</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="E88" s="0" t="s">
+      <c r="E88" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F88" s="0" t="s">
+      <c r="F88" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G88" s="0" t="s">
+      <c r="G88" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H88" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I88" s="0" t="s">
-        <v>1122</v>
-      </c>
-      <c r="K88" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L88" s="0" t="n">
+      <c r="H88" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L88" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="M88" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N88" s="0" t="s">
+      <c r="M88" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N88" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="O88" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH88" s="3" t="s">
+      <c r="O88" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH88" s="7" t="s">
         <v>386</v>
       </c>
     </row>
@@ -20379,9 +20370,6 @@
       <c r="I91" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="K91" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L91" s="0" t="n">
         <v>3</v>
       </c>
@@ -20511,9 +20499,6 @@
       <c r="I94" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="K94" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L94" s="0" t="n">
         <v>31</v>
       </c>
@@ -21231,12 +21216,6 @@
       <c r="I109" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J109" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K109" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L109" s="0" t="n">
         <v>7</v>
       </c>
@@ -21488,53 +21467,53 @@
         <v>494</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+    <row r="115" s="6" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="C115" s="0" t="n">
+      <c r="C115" s="6" t="n">
         <v>2018</v>
       </c>
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="E115" s="0" t="s">
+      <c r="E115" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F115" s="0" t="s">
+      <c r="F115" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G115" s="0" t="s">
+      <c r="G115" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H115" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I115" s="0" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J115" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K115" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L115" s="0" t="n">
+      <c r="H115" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I115" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J115" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K115" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L115" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="M115" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N115" s="0" t="s">
+      <c r="M115" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N115" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="O115" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH115" s="3" t="s">
+      <c r="O115" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH115" s="7" t="s">
         <v>498</v>
       </c>
     </row>
@@ -21940,10 +21919,10 @@
         <v>174</v>
       </c>
       <c r="J124" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K124" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L124" s="4" t="n">
         <v>175</v>
@@ -21958,50 +21937,50 @@
         <v>526</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+    <row r="125" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B125" s="0" t="s">
+      <c r="B125" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="C125" s="0" t="n">
+      <c r="C125" s="6" t="n">
         <v>2010</v>
       </c>
-      <c r="D125" s="0" t="s">
+      <c r="D125" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="E125" s="0" t="s">
+      <c r="E125" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="F125" s="0" t="s">
+      <c r="F125" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="G125" s="0" t="s">
+      <c r="G125" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H125" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I125" s="0" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J125" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K125" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L125" s="0" t="n">
+      <c r="H125" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J125" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K125" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L125" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="M125" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N125" s="0" t="s">
+      <c r="M125" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N125" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="O125" s="0" t="s">
+      <c r="O125" s="6" t="s">
         <v>155</v>
       </c>
     </row>
@@ -22466,7 +22445,7 @@
         <v>40</v>
       </c>
       <c r="K135" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L135" s="0" t="n">
         <v>2</v>
@@ -22604,10 +22583,10 @@
         <v>174</v>
       </c>
       <c r="J138" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K138" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L138" s="4" t="n">
         <v>44</v>
@@ -22744,12 +22723,6 @@
       <c r="I141" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J141" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K141" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L141" s="0" t="n">
         <v>4</v>
       </c>
@@ -22794,12 +22767,6 @@
       <c r="I142" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J142" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K142" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L142" s="0" t="n">
         <v>4</v>
       </c>
@@ -23289,7 +23256,7 @@
         <v>40</v>
       </c>
       <c r="K152" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L152" s="4" t="n">
         <v>1</v>
@@ -23461,12 +23428,6 @@
       <c r="I156" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="J156" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K156" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="157" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4" t="s">
@@ -23496,12 +23457,6 @@
       <c r="I157" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="J157" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K157" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="158" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="s">
@@ -23531,12 +23486,6 @@
       <c r="I158" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="J158" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K158" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
@@ -23793,10 +23742,10 @@
         <v>444</v>
       </c>
       <c r="J164" s="0" t="s">
-        <v>679</v>
+        <v>41</v>
       </c>
       <c r="K164" s="0" t="s">
-        <v>679</v>
+        <v>41</v>
       </c>
       <c r="L164" s="0" t="n">
         <v>42</v>
@@ -24640,10 +24589,10 @@
         <v>174</v>
       </c>
       <c r="J181" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K181" s="4" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L181" s="4" t="n">
         <v>88</v>
@@ -25344,12 +25293,6 @@
       <c r="I196" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J196" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K196" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L196" s="0" t="n">
         <v>2</v>
       </c>
@@ -25574,12 +25517,6 @@
       <c r="I200" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J200" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K200" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L200" s="0" t="n">
         <v>61</v>
       </c>
@@ -25634,50 +25571,50 @@
         <v>820</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
+    <row r="202" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B202" s="0" t="s">
+      <c r="B202" s="6" t="s">
         <v>821</v>
       </c>
-      <c r="C202" s="0" t="n">
+      <c r="C202" s="6" t="n">
         <v>2015</v>
       </c>
-      <c r="D202" s="0" t="s">
+      <c r="D202" s="6" t="s">
         <v>822</v>
       </c>
-      <c r="E202" s="0" t="s">
+      <c r="E202" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="F202" s="0" t="s">
+      <c r="F202" s="6" t="s">
         <v>823</v>
       </c>
-      <c r="G202" s="0" t="s">
+      <c r="G202" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H202" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I202" s="0" t="s">
+      <c r="H202" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I202" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="J202" s="0" t="s">
+      <c r="J202" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="K202" s="0" t="s">
+      <c r="K202" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="L202" s="0" t="n">
+      <c r="L202" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="M202" s="0" t="s">
+      <c r="M202" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="N202" s="0" t="s">
+      <c r="N202" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="O202" s="0" t="s">
+      <c r="O202" s="6" t="s">
         <v>155</v>
       </c>
     </row>
@@ -25709,12 +25646,6 @@
       <c r="I203" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="J203" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K203" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="L203" s="4" t="n">
         <v>3</v>
       </c>
@@ -26245,10 +26176,10 @@
         <v>41</v>
       </c>
       <c r="I214" s="0" t="s">
-        <v>1122</v>
+        <v>444</v>
       </c>
       <c r="J214" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K214" s="0" t="s">
         <v>40</v>
@@ -26513,7 +26444,7 @@
         <v>174</v>
       </c>
       <c r="J219" s="4" t="s">
-        <v>679</v>
+        <v>41</v>
       </c>
       <c r="K219" s="4" t="s">
         <v>40</v>
@@ -26975,7 +26906,7 @@
         <v>444</v>
       </c>
       <c r="J228" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="K228" s="0" t="s">
         <v>40</v>
@@ -27295,12 +27226,6 @@
       <c r="I234" s="0" t="s">
         <v>1122</v>
       </c>
-      <c r="J234" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K234" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L234" s="0" t="n">
         <v>21</v>
       </c>
@@ -27526,7 +27451,7 @@
         <v>40</v>
       </c>
       <c r="K238" s="0" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="L238" s="0" t="n">
         <v>178</v>

</xml_diff>

<commit_message>
Finished cleaning operationalization quotes for all studies
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10162" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10154" uniqueCount="1124">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -613,7 +613,7 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
 How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
 Haven't seen how income was meausred. 
 </t>
@@ -697,7 +697,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -784,7 +784,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -944,7 +944,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1022,7 +1022,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1044,7 +1044,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1606,7 +1606,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1658,11 +1658,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1739,26 +1739,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1875,7 +1875,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1884,12 +1884,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1914,7 +1914,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1949,9 +1949,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1984,7 +1984,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2040,8 +2040,8 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2156,7 +2156,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2215,7 +2215,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2226,7 +2226,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2272,7 +2272,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2372,7 +2372,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2520,7 +2520,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2579,7 +2579,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2621,7 +2621,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2706,7 +2706,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3089,7 +3089,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3159,19 +3159,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3299,7 +3299,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3443,7 +3443,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3613,7 +3613,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3757,7 +3757,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3826,12 +3826,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3854,7 +3854,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3894,13 +3894,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3955,14 +3955,14 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4015,7 +4015,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4090,7 +4090,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4106,6 +4106,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -4144,7 +4150,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4170,6 +4176,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4214,7 +4228,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -4269,11 +4283,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E239" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A239" activeCellId="0" sqref="A239"/>
-      <selection pane="bottomRight" activeCell="A257" activeCellId="0" sqref="257:257"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16584,11 +16598,11 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E247" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N207" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A247" activeCellId="0" sqref="A247"/>
-      <selection pane="bottomRight" activeCell="E257" activeCellId="0" sqref="257:257"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A207" activeCellId="0" sqref="A207"/>
+      <selection pane="bottomRight" activeCell="AG209" activeCellId="0" sqref="AG209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18689,53 +18703,53 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="7" t="n">
         <v>2015</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G55" s="0" t="s">
+      <c r="G55" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H55" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I55" s="0" t="s">
+      <c r="H55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J55" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K55" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L55" s="0" t="n">
+      <c r="J55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L55" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="M55" s="0" t="s">
+      <c r="M55" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="O55" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH55" s="3" t="s">
+      <c r="N55" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH55" s="8" t="s">
         <v>258</v>
       </c>
     </row>
@@ -18974,7 +18988,7 @@
         <v>287</v>
       </c>
       <c r="R60" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="S60" s="0" t="s">
         <v>288</v>
@@ -19640,9 +19654,6 @@
       <c r="L74" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N74" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="O74" s="0" t="s">
         <v>155</v>
       </c>
@@ -20013,50 +20024,50 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
+    <row r="84" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C84" s="4" t="n">
+      <c r="C84" s="7" t="n">
         <v>2006</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="F84" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="G84" s="4" t="s">
+      <c r="G84" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H84" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I84" s="4" t="s">
+      <c r="H84" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I84" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J84" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L84" s="4" t="n">
+      <c r="J84" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L84" s="7" t="n">
         <v>59</v>
       </c>
-      <c r="M84" s="4" t="s">
+      <c r="M84" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N84" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="O84" s="4" t="s">
+      <c r="N84" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O84" s="7" t="s">
         <v>155</v>
       </c>
     </row>
@@ -20235,7 +20246,7 @@
       <c r="O88" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AH88" s="7" t="s">
+      <c r="AH88" s="9" t="s">
         <v>386</v>
       </c>
     </row>
@@ -20835,53 +20846,53 @@
         <v>441</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+    <row r="102" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="C102" s="0" t="n">
+      <c r="C102" s="7" t="n">
         <v>2018</v>
       </c>
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="E102" s="0" t="s">
+      <c r="E102" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F102" s="0" t="s">
+      <c r="F102" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G102" s="0" t="s">
+      <c r="G102" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H102" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I102" s="0" t="s">
+      <c r="H102" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I102" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J102" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K102" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L102" s="0" t="n">
+      <c r="J102" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K102" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L102" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="M102" s="0" t="s">
+      <c r="M102" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="N102" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="O102" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH102" s="3" t="s">
+      <c r="N102" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O102" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH102" s="8" t="s">
         <v>446</v>
       </c>
     </row>
@@ -21078,7 +21089,7 @@
       <c r="O106" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AH106" s="7" t="s">
+      <c r="AH106" s="9" t="s">
         <v>465</v>
       </c>
     </row>
@@ -21510,7 +21521,7 @@
       <c r="O115" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AH115" s="7" t="s">
+      <c r="AH115" s="9" t="s">
         <v>498</v>
       </c>
     </row>
@@ -22406,7 +22417,7 @@
       <c r="O134" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AH134" s="7" t="s">
+      <c r="AH134" s="9" t="s">
         <v>567</v>
       </c>
     </row>
@@ -22723,9 +22734,6 @@
       <c r="L141" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="N141" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="O141" s="0" t="s">
         <v>291</v>
       </c>
@@ -22764,57 +22772,54 @@
       <c r="L142" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="N142" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="O142" s="0" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+    <row r="143" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A143" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B143" s="0" t="s">
+      <c r="B143" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="C143" s="0" t="n">
+      <c r="C143" s="7" t="n">
         <v>2018</v>
       </c>
-      <c r="D143" s="0" t="s">
+      <c r="D143" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="E143" s="0" t="s">
+      <c r="E143" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F143" s="0" t="s">
+      <c r="F143" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="G143" s="0" t="s">
+      <c r="G143" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H143" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I143" s="0" t="s">
+      <c r="H143" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I143" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J143" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K143" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L143" s="0" t="n">
+      <c r="J143" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L143" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="M143" s="0" t="s">
+      <c r="M143" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N143" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="O143" s="3" t="s">
+      <c r="N143" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O143" s="8" t="s">
         <v>598</v>
       </c>
     </row>
@@ -23607,147 +23612,147 @@
         <v>669</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+    <row r="162" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B162" s="0" t="s">
+      <c r="B162" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="C162" s="0" t="n">
+      <c r="C162" s="7" t="n">
         <v>2016</v>
       </c>
-      <c r="D162" s="0" t="s">
+      <c r="D162" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="E162" s="0" t="s">
+      <c r="E162" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="F162" s="0" t="s">
+      <c r="F162" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="G162" s="0" t="s">
+      <c r="G162" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H162" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I162" s="0" t="s">
+      <c r="H162" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I162" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J162" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K162" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L162" s="0" t="n">
+      <c r="J162" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K162" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L162" s="7" t="n">
         <v>65</v>
       </c>
-      <c r="M162" s="0" t="s">
+      <c r="M162" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N162" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="O162" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="11.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+      <c r="N162" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O162" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="163" s="7" customFormat="true" ht="11.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A163" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B163" s="0" t="s">
+      <c r="B163" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="C163" s="0" t="n">
+      <c r="C163" s="7" t="n">
         <v>2017</v>
       </c>
-      <c r="D163" s="0" t="s">
+      <c r="D163" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="E163" s="0" t="s">
+      <c r="E163" s="7" t="s">
         <v>658</v>
       </c>
-      <c r="F163" s="0" t="s">
+      <c r="F163" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="G163" s="0" t="s">
+      <c r="G163" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H163" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I163" s="0" t="s">
+      <c r="H163" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I163" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J163" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K163" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L163" s="0" t="n">
+      <c r="J163" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K163" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L163" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="M163" s="0" t="s">
+      <c r="M163" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N163" s="0" t="s">
+      <c r="N163" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="O163" s="0" t="s">
+      <c r="O163" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="AH163" s="3" t="s">
+      <c r="AH163" s="8" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+    <row r="164" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B164" s="0" t="s">
+      <c r="B164" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="C164" s="0" t="n">
+      <c r="C164" s="7" t="n">
         <v>2000</v>
       </c>
-      <c r="D164" s="0" t="s">
+      <c r="D164" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="E164" s="0" t="s">
+      <c r="E164" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="F164" s="0" t="s">
+      <c r="F164" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="G164" s="0" t="s">
+      <c r="G164" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H164" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I164" s="0" t="s">
+      <c r="H164" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I164" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J164" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K164" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L164" s="0" t="n">
+      <c r="J164" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K164" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L164" s="7" t="n">
         <v>42</v>
       </c>
-      <c r="M164" s="0" t="s">
+      <c r="M164" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N164" s="0" t="s">
+      <c r="N164" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="O164" s="0" t="s">
+      <c r="O164" s="7" t="s">
         <v>680</v>
       </c>
     </row>
@@ -24208,41 +24213,41 @@
         <v>155</v>
       </c>
     </row>
-    <row r="173" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="4" t="s">
+    <row r="173" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B173" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="C173" s="4" t="n">
+      <c r="C173" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="D173" s="4" t="s">
+      <c r="D173" s="7" t="s">
         <v>714</v>
       </c>
-      <c r="E173" s="4" t="s">
+      <c r="E173" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="F173" s="4" t="s">
+      <c r="F173" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="G173" s="4" t="s">
+      <c r="G173" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H173" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I173" s="4" t="s">
+      <c r="H173" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I173" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J173" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K173" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L173" s="4" t="n">
+      <c r="J173" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K173" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L173" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -24275,41 +24280,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="4" t="s">
+    <row r="175" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B175" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="C175" s="4" t="n">
+      <c r="C175" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="D175" s="4" t="s">
+      <c r="D175" s="7" t="s">
         <v>714</v>
       </c>
-      <c r="E175" s="4" t="s">
+      <c r="E175" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="F175" s="4" t="s">
+      <c r="F175" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="G175" s="4" t="s">
+      <c r="G175" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H175" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I175" s="4" t="s">
+      <c r="H175" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I175" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J175" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K175" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L175" s="4" t="n">
+      <c r="J175" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K175" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L175" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -24366,7 +24371,7 @@
         <v>155</v>
       </c>
       <c r="R176" s="4" t="s">
-        <v>155</v>
+        <v>1122</v>
       </c>
       <c r="S176" s="4" t="s">
         <v>155</v>
@@ -24378,53 +24383,53 @@
         <v>155</v>
       </c>
       <c r="V176" s="4" t="s">
-        <v>155</v>
+        <v>1122</v>
       </c>
       <c r="W176" s="4" t="s">
         <v>155</v>
       </c>
       <c r="X176" s="4" t="s">
-        <v>155</v>
+        <v>1122</v>
       </c>
       <c r="Y176" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="177" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="4" t="s">
+    <row r="177" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="C177" s="4" t="n">
+      <c r="C177" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="D177" s="4" t="s">
+      <c r="D177" s="7" t="s">
         <v>714</v>
       </c>
-      <c r="E177" s="4" t="s">
+      <c r="E177" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="F177" s="4" t="s">
+      <c r="F177" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="G177" s="4" t="s">
+      <c r="G177" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H177" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I177" s="4" t="s">
+      <c r="H177" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I177" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J177" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K177" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L177" s="4" t="n">
+      <c r="J177" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K177" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L177" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -25287,9 +25292,6 @@
       <c r="L196" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N196" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="O196" s="0" t="s">
         <v>633</v>
       </c>
@@ -25412,13 +25414,13 @@
         <v>155</v>
       </c>
       <c r="V198" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="W198" s="0" t="s">
         <v>288</v>
       </c>
       <c r="X198" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="Y198" s="0" t="s">
         <v>288</v>
@@ -26391,7 +26393,7 @@
         <v>291</v>
       </c>
       <c r="N218" s="4" t="s">
-        <v>898</v>
+        <v>1122</v>
       </c>
       <c r="O218" s="4" t="s">
         <v>898</v>
@@ -26444,7 +26446,7 @@
         <v>291</v>
       </c>
       <c r="N219" s="4" t="s">
-        <v>155</v>
+        <v>1122</v>
       </c>
       <c r="O219" s="4" t="s">
         <v>155</v>
@@ -26497,7 +26499,7 @@
         <v>291</v>
       </c>
       <c r="N220" s="4" t="s">
-        <v>902</v>
+        <v>1122</v>
       </c>
       <c r="O220" s="4" t="s">
         <v>902</v>
@@ -26549,8 +26551,8 @@
       <c r="M221" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="N221" s="0" t="s">
-        <v>155</v>
+      <c r="N221" s="4" t="s">
+        <v>1122</v>
       </c>
       <c r="O221" s="0" t="s">
         <v>155</v>
@@ -26559,9 +26561,6 @@
         <v>906</v>
       </c>
       <c r="Q221" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="R221" s="0" t="s">
         <v>155</v>
       </c>
       <c r="AH221" s="3" t="s">
@@ -26965,7 +26964,7 @@
         <v>287</v>
       </c>
       <c r="R229" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="S229" s="0" t="s">
         <v>288</v>
@@ -27217,19 +27216,10 @@
       <c r="L234" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="N234" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="O234" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="P234" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="Q234" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="R234" s="0" t="s">
         <v>155</v>
       </c>
       <c r="AH234" s="3" t="s">
@@ -27336,7 +27326,7 @@
         <v>983</v>
       </c>
       <c r="R236" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="S236" s="0" t="s">
         <v>288</v>
@@ -28093,53 +28083,53 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A251" s="0" t="s">
+    <row r="251" s="7" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A251" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B251" s="0" t="s">
+      <c r="B251" s="7" t="s">
         <v>1052</v>
       </c>
-      <c r="C251" s="0" t="n">
+      <c r="C251" s="7" t="n">
         <v>2013</v>
       </c>
-      <c r="D251" s="0" t="s">
+      <c r="D251" s="7" t="s">
         <v>1053</v>
       </c>
-      <c r="E251" s="0" t="s">
+      <c r="E251" s="7" t="s">
         <v>1054</v>
       </c>
-      <c r="F251" s="0" t="s">
+      <c r="F251" s="7" t="s">
         <v>1055</v>
       </c>
-      <c r="G251" s="0" t="s">
+      <c r="G251" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H251" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I251" s="0" t="s">
+      <c r="H251" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I251" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J251" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K251" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L251" s="0" t="n">
+      <c r="J251" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K251" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L251" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="M251" s="0" t="s">
+      <c r="M251" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N251" s="3" t="s">
+      <c r="N251" s="8" t="s">
         <v>1056</v>
       </c>
-      <c r="O251" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH251" s="3" t="s">
+      <c r="O251" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH251" s="8" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -28193,53 +28183,53 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A253" s="0" t="s">
+    <row r="253" s="7" customFormat="true" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A253" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B253" s="0" t="s">
+      <c r="B253" s="7" t="s">
         <v>1062</v>
       </c>
-      <c r="C253" s="0" t="n">
+      <c r="C253" s="7" t="n">
         <v>2017</v>
       </c>
-      <c r="D253" s="0" t="s">
+      <c r="D253" s="7" t="s">
         <v>1063</v>
       </c>
-      <c r="E253" s="0" t="s">
+      <c r="E253" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F253" s="0" t="s">
+      <c r="F253" s="7" t="s">
         <v>1064</v>
       </c>
-      <c r="G253" s="0" t="s">
+      <c r="G253" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H253" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I253" s="0" t="s">
+      <c r="H253" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I253" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="J253" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K253" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L253" s="0" t="n">
+      <c r="J253" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K253" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L253" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M253" s="0" t="s">
+      <c r="M253" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N253" s="0" t="s">
+      <c r="N253" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="O253" s="0" t="s">
+      <c r="O253" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="AH253" s="3" t="s">
+      <c r="AH253" s="8" t="s">
         <v>1065</v>
       </c>
     </row>
@@ -28343,13 +28333,13 @@
         <v>291</v>
       </c>
       <c r="N255" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="O255" s="0" t="s">
         <v>288</v>
       </c>
       <c r="P255" s="0" t="s">
-        <v>288</v>
+        <v>1122</v>
       </c>
       <c r="Q255" s="0" t="s">
         <v>288</v>
@@ -28463,10 +28453,10 @@
       <c r="L257" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="P257" s="7" t="s">
+      <c r="P257" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="Q257" s="7" t="s">
+      <c r="Q257" s="9" t="s">
         <v>1089</v>
       </c>
       <c r="AH257" s="5" t="s">
@@ -28789,7 +28779,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
-      <selection pane="bottomRight" activeCell="B15" activeCellId="1" sqref="257:257 B15"/>
+      <selection pane="bottomRight" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Finished coding reasons for operationalizations
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10158" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10152" uniqueCount="1124">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -613,7 +613,7 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
 How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
 Haven't seen how income was meausred. 
 </t>
@@ -697,7 +697,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -784,7 +784,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -944,7 +944,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1022,7 +1022,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1044,7 +1044,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1609,7 +1609,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1661,11 +1661,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1742,26 +1742,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1878,7 +1878,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1887,12 +1887,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1917,7 +1917,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1952,9 +1952,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1987,7 +1987,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2043,8 +2043,8 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2159,7 +2159,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2218,7 +2218,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2229,7 +2229,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2275,7 +2275,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2375,7 +2375,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2523,7 +2523,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2582,7 +2582,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2624,7 +2624,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2709,7 +2709,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3092,7 +3092,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3162,19 +3162,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3302,7 +3302,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3446,7 +3446,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3616,7 +3616,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3760,7 +3760,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3829,12 +3829,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3857,7 +3857,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3897,13 +3897,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3958,14 +3958,14 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4018,7 +4018,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4150,7 +4150,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4189,6 +4189,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4282,7 +4286,7 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -16603,12 +16607,12 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
-      <selection pane="bottomRight" activeCell="I78" activeCellId="0" sqref="I78"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="AC23" activeCellId="0" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17760,7 +17764,7 @@
         <v>172</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17807,7 +17811,7 @@
         <v>176</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17854,7 +17858,7 @@
         <v>179</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18215,7 +18219,7 @@
         <v>219</v>
       </c>
       <c r="Q44" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18268,7 +18272,7 @@
         <v>219</v>
       </c>
       <c r="Q45" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18321,7 +18325,7 @@
         <v>219</v>
       </c>
       <c r="Q46" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18465,7 +18469,7 @@
         <v>235</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18512,7 +18516,7 @@
         <v>240</v>
       </c>
       <c r="O50" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH50" s="3" t="s">
         <v>241</v>
@@ -18562,7 +18566,7 @@
         <v>245</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18609,7 +18613,7 @@
         <v>246</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18656,7 +18660,7 @@
         <v>249</v>
       </c>
       <c r="O53" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18703,7 +18707,7 @@
         <v>253</v>
       </c>
       <c r="O54" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH54" s="0" t="s">
         <v>254</v>
@@ -18753,7 +18757,7 @@
         <v>155</v>
       </c>
       <c r="O55" s="7" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH55" s="8" t="s">
         <v>258</v>
@@ -18885,7 +18889,7 @@
         <v>272</v>
       </c>
       <c r="O58" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH58" s="0" t="s">
         <v>273</v>
@@ -18935,7 +18939,7 @@
         <v>278</v>
       </c>
       <c r="O59" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH59" s="0" t="s">
         <v>279</v>
@@ -18997,7 +19001,7 @@
         <v>356</v>
       </c>
       <c r="S60" s="0" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19185,7 +19189,7 @@
         <v>301</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19232,7 +19236,7 @@
         <v>304</v>
       </c>
       <c r="O65" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19279,7 +19283,7 @@
         <v>308</v>
       </c>
       <c r="O66" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH66" s="0" t="s">
         <v>309</v>
@@ -19329,7 +19333,7 @@
         <v>313</v>
       </c>
       <c r="O67" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH67" s="0" t="s">
         <v>314</v>
@@ -19379,7 +19383,7 @@
         <v>319</v>
       </c>
       <c r="O68" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH68" s="3" t="s">
         <v>320</v>
@@ -19429,106 +19433,106 @@
         <v>323</v>
       </c>
       <c r="O69" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH69" s="0" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G70" s="0" t="s">
+      <c r="G70" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H70" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="0" t="s">
+      <c r="H70" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I70" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="J70" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K70" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L70" s="0" t="n">
+      <c r="J70" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L70" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="M70" s="0" t="s">
+      <c r="M70" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="N70" s="0" t="s">
+      <c r="N70" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="O70" s="0" t="s">
+      <c r="O70" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="AH70" s="3" t="s">
+      <c r="AH70" s="6" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="F71" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G71" s="0" t="s">
+      <c r="G71" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H71" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I71" s="0" t="s">
+      <c r="H71" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I71" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="J71" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L71" s="0" t="n">
+      <c r="J71" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L71" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="M71" s="0" t="s">
+      <c r="M71" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="N71" s="0" t="s">
+      <c r="N71" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="O71" s="0" t="s">
+      <c r="O71" s="4" t="s">
         <v>331</v>
       </c>
     </row>
@@ -19576,7 +19580,7 @@
         <v>336</v>
       </c>
       <c r="O72" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH72" s="3" t="s">
         <v>337</v>
@@ -19626,7 +19630,7 @@
         <v>340</v>
       </c>
       <c r="O73" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19660,9 +19664,6 @@
       <c r="L74" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O74" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="AH74" s="0" t="s">
         <v>344</v>
       </c>
@@ -19810,7 +19811,7 @@
         <v>359</v>
       </c>
       <c r="O78" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19904,7 +19905,7 @@
         <v>367</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
     </row>
     <row r="81" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19951,7 +19952,7 @@
         <v>367</v>
       </c>
       <c r="O81" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20077,7 +20078,7 @@
         <v>155</v>
       </c>
       <c r="O84" s="7" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="85" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20156,7 +20157,7 @@
         <v>376</v>
       </c>
       <c r="O86" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH86" s="0" t="s">
         <v>377</v>
@@ -20253,7 +20254,7 @@
         <v>386</v>
       </c>
       <c r="O88" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH88" s="9" t="s">
         <v>387</v>
@@ -20438,7 +20439,7 @@
         <v>406</v>
       </c>
       <c r="O92" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20485,7 +20486,7 @@
         <v>409</v>
       </c>
       <c r="O93" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20755,7 +20756,7 @@
         <v>434</v>
       </c>
       <c r="O99" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH99" s="6" t="s">
         <v>435</v>
@@ -20899,7 +20900,7 @@
         <v>155</v>
       </c>
       <c r="O102" s="7" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH102" s="8" t="s">
         <v>447</v>
@@ -20996,7 +20997,7 @@
         <v>455</v>
       </c>
       <c r="O104" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH104" s="3" t="s">
         <v>456</v>
@@ -21096,7 +21097,7 @@
         <v>465</v>
       </c>
       <c r="O106" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH106" s="9" t="s">
         <v>466</v>
@@ -21152,7 +21153,7 @@
         <v>471</v>
       </c>
       <c r="Q107" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH107" s="0" t="s">
         <v>472</v>
@@ -21202,7 +21203,7 @@
         <v>475</v>
       </c>
       <c r="O108" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21281,7 +21282,7 @@
         <v>480</v>
       </c>
       <c r="O110" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH110" s="0" t="s">
         <v>481</v>
@@ -21381,7 +21382,7 @@
         <v>490</v>
       </c>
       <c r="O112" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH112" s="4" t="s">
         <v>491</v>
@@ -21431,7 +21432,7 @@
         <v>492</v>
       </c>
       <c r="O113" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="114" s="4" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21528,7 +21529,7 @@
         <v>498</v>
       </c>
       <c r="O115" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH115" s="9" t="s">
         <v>499</v>
@@ -21578,7 +21579,7 @@
         <v>502</v>
       </c>
       <c r="O116" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH116" s="0" t="s">
         <v>503</v>
@@ -21998,7 +21999,7 @@
         <v>530</v>
       </c>
       <c r="O125" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22045,7 +22046,7 @@
         <v>533</v>
       </c>
       <c r="O126" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH126" s="0" t="s">
         <v>534</v>
@@ -22230,7 +22231,7 @@
         <v>548</v>
       </c>
       <c r="O130" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH130" s="3" t="s">
         <v>549</v>
@@ -22377,7 +22378,7 @@
         <v>563</v>
       </c>
       <c r="O133" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="134" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22424,7 +22425,7 @@
         <v>567</v>
       </c>
       <c r="O134" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH134" s="9" t="s">
         <v>568</v>
@@ -22568,7 +22569,7 @@
         <v>579</v>
       </c>
       <c r="O137" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="138" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22662,7 +22663,7 @@
         <v>585</v>
       </c>
       <c r="O139" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22743,9 +22744,6 @@
       <c r="L141" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="O141" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="AH141" s="3" t="s">
         <v>593</v>
       </c>
@@ -22781,9 +22779,6 @@
       <c r="L142" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="O142" s="0" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="143" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="7" t="s">
@@ -22876,7 +22871,7 @@
         <v>602</v>
       </c>
       <c r="O144" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH144" s="0" t="s">
         <v>603</v>
@@ -23073,7 +23068,7 @@
         <v>621</v>
       </c>
       <c r="O148" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH148" s="3" t="s">
         <v>622</v>
@@ -23123,13 +23118,13 @@
         <v>626</v>
       </c>
       <c r="O149" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="P149" s="0" t="s">
         <v>627</v>
       </c>
       <c r="Q149" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH149" s="3" t="s">
         <v>628</v>
@@ -23273,7 +23268,7 @@
         <v>636</v>
       </c>
       <c r="O152" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="11.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23320,7 +23315,7 @@
         <v>642</v>
       </c>
       <c r="O153" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH153" s="3" t="s">
         <v>643</v>
@@ -23402,7 +23397,7 @@
         <v>651</v>
       </c>
       <c r="O155" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH155" s="0" t="s">
         <v>652</v>
@@ -23539,7 +23534,7 @@
         <v>661</v>
       </c>
       <c r="O159" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23668,7 +23663,7 @@
         <v>155</v>
       </c>
       <c r="O162" s="7" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="163" s="7" customFormat="true" ht="11.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23862,7 +23857,7 @@
         <v>688</v>
       </c>
       <c r="O166" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24074,25 +24069,25 @@
         <v>709</v>
       </c>
       <c r="O170" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="P170" s="4" t="s">
         <v>710</v>
       </c>
       <c r="Q170" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="R170" s="4" t="s">
         <v>711</v>
       </c>
       <c r="S170" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="T170" s="4" t="s">
         <v>712</v>
       </c>
       <c r="U170" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="171" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24139,25 +24134,25 @@
         <v>709</v>
       </c>
       <c r="O171" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="P171" s="4" t="s">
         <v>710</v>
       </c>
       <c r="Q171" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="R171" s="4" t="s">
         <v>711</v>
       </c>
       <c r="S171" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="T171" s="4" t="s">
         <v>712</v>
       </c>
       <c r="U171" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="172" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24204,25 +24199,25 @@
         <v>709</v>
       </c>
       <c r="O172" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="P172" s="4" t="s">
         <v>710</v>
       </c>
       <c r="Q172" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="R172" s="4" t="s">
         <v>711</v>
       </c>
       <c r="S172" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="T172" s="4" t="s">
         <v>712</v>
       </c>
       <c r="U172" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="173" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24330,81 +24325,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="4" t="s">
+    <row r="176" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="C176" s="4" t="n">
+      <c r="C176" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="D176" s="4" t="s">
+      <c r="D176" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="E176" s="4" t="s">
+      <c r="E176" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="F176" s="4" t="s">
+      <c r="F176" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="G176" s="4" t="s">
+      <c r="G176" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H176" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I176" s="4" t="s">
+      <c r="H176" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I176" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="J176" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K176" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L176" s="4" t="n">
+      <c r="J176" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K176" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L176" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M176" s="4" t="s">
+      <c r="M176" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="N176" s="4" t="s">
+      <c r="N176" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="O176" s="4" t="s">
+      <c r="O176" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="P176" s="4" t="s">
+      <c r="P176" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="Q176" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="R176" s="4" t="s">
+      <c r="Q176" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="R176" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="S176" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="T176" s="6" t="s">
+      <c r="S176" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="T176" s="9" t="s">
         <v>724</v>
       </c>
-      <c r="U176" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="V176" s="4" t="s">
+      <c r="U176" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="V176" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="W176" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="X176" s="4" t="s">
+      <c r="W176" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="Y176" s="4" t="s">
-        <v>155</v>
+      <c r="X176" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y176" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="177" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24518,7 +24513,7 @@
         <v>729</v>
       </c>
       <c r="O179" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="180" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24612,7 +24607,7 @@
         <v>732</v>
       </c>
       <c r="O181" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24709,7 +24704,7 @@
         <v>740</v>
       </c>
       <c r="O183" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24923,13 +24918,13 @@
         <v>761</v>
       </c>
       <c r="O188" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="P188" s="0" t="s">
         <v>762</v>
       </c>
       <c r="Q188" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH188" s="0" t="s">
         <v>763</v>
@@ -25079,7 +25074,7 @@
         <v>779</v>
       </c>
       <c r="O191" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
     </row>
     <row r="192" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25126,7 +25121,7 @@
         <v>779</v>
       </c>
       <c r="O192" s="4" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
     </row>
     <row r="193" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25173,7 +25168,7 @@
         <v>779</v>
       </c>
       <c r="O193" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25220,7 +25215,7 @@
         <v>784</v>
       </c>
       <c r="O194" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH194" s="3" t="s">
         <v>785</v>
@@ -25304,9 +25299,6 @@
       <c r="L196" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="O196" s="0" t="s">
-        <v>634</v>
-      </c>
       <c r="AH196" s="3" t="s">
         <v>792</v>
       </c>
@@ -25423,7 +25415,7 @@
         <v>806</v>
       </c>
       <c r="U198" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="V198" s="0" t="s">
         <v>356</v>
@@ -25617,7 +25609,7 @@
         <v>825</v>
       </c>
       <c r="O202" s="5" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="203" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25778,7 +25770,7 @@
         <v>839</v>
       </c>
       <c r="O206" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH206" s="3" t="s">
         <v>840</v>
@@ -25828,7 +25820,7 @@
         <v>844</v>
       </c>
       <c r="O207" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH207" s="0" t="s">
         <v>845</v>
@@ -26146,7 +26138,7 @@
         <v>876</v>
       </c>
       <c r="O213" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH213" s="0" t="s">
         <v>877</v>
@@ -26408,13 +26400,13 @@
         <v>356</v>
       </c>
       <c r="O218" s="4" t="s">
-        <v>899</v>
+        <v>356</v>
       </c>
       <c r="P218" s="4" t="s">
         <v>900</v>
       </c>
       <c r="Q218" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="219" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26461,13 +26453,13 @@
         <v>356</v>
       </c>
       <c r="O219" s="4" t="s">
-        <v>155</v>
+        <v>356</v>
       </c>
       <c r="P219" s="4" t="s">
         <v>901</v>
       </c>
       <c r="Q219" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="220" s="4" customFormat="true" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26514,13 +26506,13 @@
         <v>356</v>
       </c>
       <c r="O220" s="4" t="s">
-        <v>903</v>
+        <v>356</v>
       </c>
       <c r="P220" s="6" t="s">
         <v>904</v>
       </c>
       <c r="Q220" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26563,17 +26555,17 @@
       <c r="M221" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="N221" s="4" t="s">
+      <c r="N221" s="10" t="s">
         <v>356</v>
       </c>
       <c r="O221" s="0" t="s">
-        <v>155</v>
+        <v>356</v>
       </c>
       <c r="P221" s="0" t="s">
         <v>907</v>
       </c>
       <c r="Q221" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH221" s="3" t="s">
         <v>908</v>
@@ -26623,7 +26615,7 @@
         <v>911</v>
       </c>
       <c r="O222" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="223" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26717,7 +26709,7 @@
         <v>916</v>
       </c>
       <c r="O224" s="4" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH224" s="6" t="s">
         <v>917</v>
@@ -26773,19 +26765,19 @@
         <v>923</v>
       </c>
       <c r="Q225" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="R225" s="0" t="s">
         <v>924</v>
       </c>
       <c r="S225" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="T225" s="0" t="s">
         <v>925</v>
       </c>
       <c r="U225" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH225" s="3" t="s">
         <v>926</v>
@@ -26979,7 +26971,7 @@
         <v>356</v>
       </c>
       <c r="S229" s="0" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
       <c r="T229" s="0" t="s">
         <v>946</v>
@@ -27191,7 +27183,7 @@
         <v>970</v>
       </c>
       <c r="O233" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH233" s="3" t="s">
         <v>971</v>
@@ -27228,12 +27220,6 @@
       <c r="L234" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="O234" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q234" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="AH234" s="3" t="s">
         <v>974</v>
       </c>
@@ -27341,7 +27327,7 @@
         <v>356</v>
       </c>
       <c r="S236" s="0" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27450,7 +27436,7 @@
         <v>999</v>
       </c>
       <c r="O238" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH238" s="0" t="s">
         <v>1000</v>
@@ -27500,7 +27486,7 @@
         <v>1003</v>
       </c>
       <c r="O239" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH239" s="3" t="s">
         <v>1004</v>
@@ -27550,7 +27536,7 @@
         <v>1007</v>
       </c>
       <c r="O240" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH240" s="3" t="s">
         <v>1008</v>
@@ -28045,7 +28031,7 @@
         <v>1048</v>
       </c>
       <c r="O249" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28139,7 +28125,7 @@
         <v>1057</v>
       </c>
       <c r="O251" s="7" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH251" s="8" t="s">
         <v>1058</v>
@@ -28189,7 +28175,7 @@
         <v>1061</v>
       </c>
       <c r="O252" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="AH252" s="3" t="s">
         <v>1062</v>
@@ -28239,7 +28225,7 @@
         <v>291</v>
       </c>
       <c r="O253" s="7" t="s">
-        <v>634</v>
+        <v>291</v>
       </c>
       <c r="AH253" s="8" t="s">
         <v>1066</v>
@@ -28348,13 +28334,13 @@
         <v>356</v>
       </c>
       <c r="O255" s="0" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
       <c r="P255" s="0" t="s">
         <v>356</v>
       </c>
       <c r="Q255" s="0" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
       <c r="R255" s="0" t="s">
         <v>1078</v>
@@ -28631,19 +28617,19 @@
         <v>1107</v>
       </c>
       <c r="O260" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="P260" s="3" t="s">
         <v>1108</v>
       </c>
       <c r="Q260" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
       <c r="R260" s="0" t="s">
         <v>1109</v>
       </c>
       <c r="S260" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28690,7 +28676,7 @@
         <v>1113</v>
       </c>
       <c r="O261" s="0" t="s">
-        <v>155</v>
+        <v>291</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28786,7 +28772,7 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>

</xml_diff>

<commit_message>
First round of resolutions; stopped at Preacher et al., 2016 (row 162)
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13502" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13485" uniqueCount="1129">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -615,7 +615,7 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV and V (working class and poor) to those in Classes II and III". p.151
 How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
 Haven't seen how income was meausred. 
 </t>
@@ -699,7 +699,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -786,7 +786,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -946,7 +946,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1024,7 +1024,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1046,7 +1046,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1611,7 +1611,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1663,11 +1663,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1744,26 +1744,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1880,7 +1880,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1889,12 +1889,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1919,7 +1919,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1954,9 +1954,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1989,7 +1989,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2045,8 +2045,8 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2161,7 +2161,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2220,7 +2220,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2231,7 +2231,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2277,7 +2277,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2377,7 +2377,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2525,7 +2525,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2584,7 +2584,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2626,7 +2626,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2711,7 +2711,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3094,7 +3094,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3164,19 +3164,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3304,7 +3304,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3448,7 +3448,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3618,7 +3618,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3762,7 +3762,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3831,12 +3831,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3859,7 +3859,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3899,13 +3899,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3960,14 +3960,14 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4020,7 +4020,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4051,6 +4051,44 @@
   </si>
   <si>
     <t xml:space="preserve">None givne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“For the two samples taken together, parent educationand income were combined in a composite score of SES. Thecomposite was generated using principal components analysis. Thefirst principal component weighted education and income posi-tively and equally and accounted for 81% of the original variance.” p. 164</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Guardians were asked to fill out a short survey assessing
+their economic status. Family yearly income was assessed on a
+scale ranging from less than $5,000 and to over $200,000, with the
+highest number in the circled range recorded as the family’s
+income. Guardians were also asked about their occupation and
+educational attainment. (pg. 3); </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">additionally, used partial least squares to composite income and education as weighted indicators of SES—kind of a formative approach, a non-causal indicator approach (p. 196–197, 199)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">none given for indicators; “Partial least squares modeling isideal  for  examining  all  of  the  possible  associations  between  thevariables of interest as it can be used with small data sets and isrecommended  for  exploratory  purposes,  as  it  does  not  have  thestrict measurement and distributional requirements of other mod-eling procedure” (p. 194); “The partial least squares analysis algorithm simultaneously modelsthe  structural  paths  and  the  measurement  paths  and  allows  eachindicator to vary in how much it contributes to the latent variablecomposite score such that indicators with stronger relationships tothe  related  indicators  and  the  latent  construct  are  given  higherweightings.” (p. 196)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood... Research has shown a strong relationship between increased economic inequality and elevated mortality rates among the dis- advantaged and points to the contribution of rank to health in- equality (e.g., Kawachi &amp; Kennedy, 1997). To the extent that relative rank is important in this relationship, subjective percep- tions of SES are likely to be powerful predictors of health and well-being... For instance, even after accounting for effects due to objective indicators of SES (e.g., education, income), SSS uniquely predicts self-rated global health (Adler et al., 2000; Franzini &amp; Fernandez-Esquer, 2006; Hyde &amp; Jones, 2007; Ostrove, Adler, Kuppermann, &amp; Washing- ton, 2000), and negative affect (Adler et al., 2000; Ghaed &amp; Gallo, 2007; Gianaros et al., 2007; Operario et al., 2004)." (p. 138); none given for objective indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Control  variables:  Social  class  and  health  risk  factors….Demographic con-trols included level of education (8th grade thru post graduatestudy), age (in years), weekly income (in dollars) and work status(1_x0006_employed).” p. 1998</t>
   </si>
 </sst>
 </file>
@@ -4060,7 +4098,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4091,8 +4129,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4115,6 +4159,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor rgb="FF99CC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -4152,7 +4208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4193,7 +4249,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4218,7 +4298,7 @@
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF00000A"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
@@ -4249,7 +4329,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66FF66"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -4292,12 +4372,12 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="J107" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
-      <selection pane="bottomRight" activeCell="I78" activeCellId="0" sqref="I78"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
+      <selection pane="bottomRight" activeCell="E127" activeCellId="0" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16613,7 +16693,7 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
@@ -26561,7 +26641,7 @@
       <c r="M221" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="N221" s="10" t="s">
+      <c r="N221" s="2" t="s">
         <v>356</v>
       </c>
       <c r="O221" s="0" t="s">
@@ -28778,12 +28858,12 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="I143" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="Q26" activeCellId="0" sqref="Q26"/>
+      <selection pane="bottomLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
+      <selection pane="bottomRight" activeCell="J163" activeCellId="0" sqref="J163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29891,50 +29971,50 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+    <row r="34" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="10" t="n">
         <v>2004</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="H34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L34" s="4" t="n">
+      <c r="J34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="10" t="n">
         <v>42</v>
       </c>
-      <c r="M34" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N34" s="4" t="s">
+      <c r="M34" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N34" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="O34" s="4" t="s">
+      <c r="O34" s="10" t="s">
         <v>291</v>
       </c>
     </row>
@@ -29985,50 +30065,50 @@
         <v>291</v>
       </c>
     </row>
-    <row r="36" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+    <row r="36" s="7" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="4" t="n">
+      <c r="C36" s="7" t="n">
         <v>2004</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="H36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L36" s="4" t="n">
+      <c r="J36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="7" t="n">
         <v>42</v>
       </c>
-      <c r="M36" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N36" s="6" t="s">
+      <c r="M36" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="N36" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="O36" s="4" t="s">
+      <c r="O36" s="7" t="s">
         <v>291</v>
       </c>
     </row>
@@ -30096,150 +30176,150 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" s="4" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+    <row r="39" s="11" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C39" s="4" t="n">
+      <c r="C39" s="11" t="n">
         <v>2009</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="4" t="s">
+      <c r="H39" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="J39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L39" s="4" t="n">
+      <c r="J39" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="11" t="n">
         <v>55</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="N39" s="6" t="s">
+      <c r="N39" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="O39" s="6" t="s">
+      <c r="O39" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="AH39" s="6" t="s">
+      <c r="AH39" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="40" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+    <row r="40" s="10" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C40" s="4" t="n">
+      <c r="C40" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="4" t="s">
+      <c r="H40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L40" s="4" t="n">
+      <c r="J40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="M40" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N40" s="4" t="s">
+      <c r="M40" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N40" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="O40" s="4" t="s">
+      <c r="O40" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="AH40" s="6" t="s">
+      <c r="AH40" s="13" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="41" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+    <row r="41" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C41" s="4" t="n">
+      <c r="C41" s="5" t="n">
         <v>2008</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="4" t="s">
+      <c r="H41" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J41" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L41" s="4" t="n">
+      <c r="J41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L41" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="M41" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N41" s="6" t="s">
+      <c r="M41" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N41" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="O41" s="4" t="s">
+      <c r="O41" s="5" t="s">
         <v>202</v>
       </c>
     </row>
@@ -30340,162 +30420,162 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+    <row r="44" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="4" t="n">
+      <c r="C44" s="5" t="n">
         <v>2005</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I44" s="4" t="s">
+      <c r="H44" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J44" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L44" s="4" t="n">
+      <c r="J44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L44" s="5" t="n">
         <v>344</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N44" s="4" t="s">
+      <c r="M44" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N44" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O44" s="4" t="s">
+      <c r="O44" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="P44" s="4" t="s">
+      <c r="P44" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="Q44" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="45" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
+      <c r="Q44" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="C45" s="4" t="n">
+      <c r="C45" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I45" s="4" t="s">
+      <c r="H45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I45" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J45" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L45" s="4" t="n">
+      <c r="J45" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K45" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L45" s="10" t="n">
         <v>344</v>
       </c>
-      <c r="M45" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N45" s="4" t="s">
+      <c r="M45" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N45" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="O45" s="4" t="s">
+      <c r="O45" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="P45" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="Q45" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="46" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="Q45" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C46" s="4" t="n">
+      <c r="C46" s="5" t="n">
         <v>2005</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I46" s="4" t="s">
+      <c r="H46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I46" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J46" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L46" s="4" t="n">
+      <c r="J46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L46" s="5" t="n">
         <v>344</v>
       </c>
-      <c r="M46" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N46" s="4" t="s">
+      <c r="M46" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N46" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O46" s="4" t="s">
+      <c r="O46" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="P46" s="4" t="s">
+      <c r="P46" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="Q46" s="4" t="s">
+      <c r="Q46" s="5" t="s">
         <v>291</v>
       </c>
     </row>
@@ -30693,144 +30773,144 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+    <row r="51" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C51" s="4" t="n">
+      <c r="C51" s="5" t="n">
         <v>2013</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G51" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I51" s="4" t="s">
+      <c r="H51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J51" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L51" s="4" t="n">
+      <c r="J51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L51" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="M51" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N51" s="4" t="s">
+      <c r="M51" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N51" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="O51" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="52" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+      <c r="O51" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="52" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C52" s="4" t="n">
+      <c r="C52" s="5" t="n">
         <v>2013</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G52" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H52" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I52" s="4" t="s">
+      <c r="H52" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L52" s="4" t="n">
+      <c r="J52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L52" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="M52" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N52" s="4" t="s">
+      <c r="M52" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N52" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="O52" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="53" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
+      <c r="O52" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" s="10" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C53" s="4" t="n">
+      <c r="C53" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G53" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="H53" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L53" s="4" t="n">
+      <c r="J53" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L53" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="M53" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N53" s="6" t="s">
+      <c r="M53" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N53" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="O53" s="4" t="s">
+      <c r="O53" s="10" t="s">
         <v>291</v>
       </c>
     </row>
@@ -30884,53 +30964,38 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
+    <row r="55" s="14" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="C55" s="7" t="n">
+      <c r="C55" s="14" t="n">
         <v>2015</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F55" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G55" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="J55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L55" s="7" t="n">
+      <c r="H55" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="L55" s="14" t="n">
         <v>27</v>
       </c>
-      <c r="M55" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="N55" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="O55" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH55" s="8" t="s">
+      <c r="AH55" s="15" t="s">
         <v>258</v>
       </c>
     </row>
@@ -31225,141 +31290,141 @@
         <v>293</v>
       </c>
     </row>
-    <row r="62" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
+    <row r="62" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C62" s="4" t="n">
+      <c r="C62" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H62" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I62" s="4" t="s">
+      <c r="H62" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I62" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J62" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L62" s="4" t="n">
+      <c r="J62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L62" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M62" s="4" t="s">
+      <c r="M62" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="N62" s="4" t="s">
+      <c r="N62" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="63" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
+    <row r="63" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C63" s="4" t="n">
+      <c r="C63" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H63" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I63" s="4" t="s">
+      <c r="H63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I63" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J63" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L63" s="4" t="n">
+      <c r="J63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L63" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M63" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N63" s="4" t="s">
+      <c r="M63" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N63" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="O63" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="64" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="O63" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="64" s="10" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="4" t="n">
+      <c r="C64" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="G64" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H64" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I64" s="4" t="s">
+      <c r="H64" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I64" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L64" s="4" t="n">
+      <c r="J64" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L64" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="M64" s="6" t="s">
+      <c r="M64" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="6" t="s">
+      <c r="N64" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="O64" s="4" t="s">
+      <c r="O64" s="10" t="s">
         <v>291</v>
       </c>
     </row>
@@ -31610,100 +31675,100 @@
         <v>324</v>
       </c>
     </row>
-    <row r="70" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
+    <row r="70" s="10" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="C70" s="4" t="n">
+      <c r="C70" s="10" t="n">
         <v>2017</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F70" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H70" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="4" t="s">
+      <c r="H70" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I70" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J70" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L70" s="4" t="n">
+      <c r="J70" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L70" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="M70" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N70" s="4" t="s">
+      <c r="M70" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N70" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="O70" s="4" t="s">
+      <c r="O70" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="AH70" s="6" t="s">
+      <c r="AH70" s="13" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="71" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
+    <row r="71" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="C71" s="4" t="n">
+      <c r="C71" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="G71" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H71" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I71" s="4" t="s">
+      <c r="H71" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I71" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="J71" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K71" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L71" s="4" t="n">
+      <c r="J71" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L71" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M71" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N71" s="4" t="s">
+      <c r="M71" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N71" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="O71" s="4" t="s">
+      <c r="O71" s="5" t="s">
         <v>331</v>
       </c>
     </row>
@@ -32032,176 +32097,176 @@
         <v>363</v>
       </c>
     </row>
-    <row r="80" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="s">
+    <row r="80" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="C80" s="4" t="n">
+      <c r="C80" s="5" t="n">
         <v>2003</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F80" s="4" t="s">
+      <c r="F80" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="G80" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H80" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I80" s="4" t="s">
+      <c r="H80" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I80" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J80" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L80" s="4" t="n">
+      <c r="J80" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L80" s="5" t="n">
         <v>114</v>
       </c>
-      <c r="M80" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N80" s="4" t="s">
+      <c r="M80" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N80" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="O80" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="81" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="s">
+      <c r="O80" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="81" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="C81" s="4" t="n">
+      <c r="C81" s="10" t="n">
         <v>2003</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="F81" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H81" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I81" s="4" t="s">
+      <c r="H81" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I81" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J81" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L81" s="4" t="n">
+      <c r="J81" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K81" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L81" s="10" t="n">
         <v>114</v>
       </c>
-      <c r="M81" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N81" s="4" t="s">
+      <c r="M81" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N81" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="O81" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="82" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
+      <c r="O81" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="82" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="C82" s="4" t="n">
+      <c r="C82" s="5" t="n">
         <v>2003</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F82" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H82" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I82" s="4" t="s">
+      <c r="H82" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J82" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L82" s="4" t="n">
+      <c r="J82" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K82" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L82" s="5" t="n">
         <v>114</v>
       </c>
-      <c r="M82" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N82" s="4" t="s">
+      <c r="M82" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N82" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="O82" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="83" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
+      <c r="O82" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="C83" s="4" t="n">
+      <c r="C83" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="F83" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="G83" s="4" t="s">
+      <c r="G83" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H83" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I83" s="4" t="s">
+      <c r="H83" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I83" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="L83" s="4" t="n">
+      <c r="L83" s="10" t="n">
         <v>59</v>
       </c>
     </row>
@@ -32231,56 +32296,41 @@
         <v>41</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="J84" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K84" s="7" t="s">
-        <v>41</v>
+        <v>356</v>
       </c>
       <c r="L84" s="7" t="n">
         <v>59</v>
       </c>
-      <c r="M84" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="N84" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="O84" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="85" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
+    </row>
+    <row r="85" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="C85" s="4" t="n">
+      <c r="C85" s="5" t="n">
         <v>2006</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="G85" s="4" t="s">
+      <c r="G85" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H85" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I85" s="4" t="s">
+      <c r="H85" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I85" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="L85" s="4" t="n">
+      <c r="L85" s="5" t="n">
         <v>59</v>
       </c>
     </row>
@@ -32381,53 +32431,53 @@
         <v>383</v>
       </c>
     </row>
-    <row r="88" s="5" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
+    <row r="88" s="14" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="C88" s="5" t="n">
+      <c r="C88" s="14" t="n">
         <v>2015</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="14" t="s">
         <v>385</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="G88" s="5" t="s">
+      <c r="G88" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H88" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L88" s="5" t="n">
+      <c r="H88" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I88" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J88" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K88" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L88" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="M88" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH88" s="9" t="s">
+      <c r="M88" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N88" s="16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH88" s="15" t="s">
         <v>387</v>
       </c>
     </row>
@@ -32883,100 +32933,100 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4" t="s">
+    <row r="99" s="10" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C99" s="4" t="n">
+      <c r="C99" s="10" t="n">
         <v>2000</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="E99" s="4" t="s">
+      <c r="E99" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="F99" s="4" t="s">
+      <c r="F99" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G99" s="4" t="s">
+      <c r="G99" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H99" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I99" s="4" t="s">
+      <c r="H99" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I99" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J99" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K99" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L99" s="4" t="n">
+      <c r="J99" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K99" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L99" s="10" t="n">
         <v>453</v>
       </c>
-      <c r="M99" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N99" s="4" t="s">
+      <c r="M99" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N99" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="O99" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH99" s="6" t="s">
+      <c r="O99" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH99" s="13" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="100" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4" t="s">
+    <row r="100" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="C100" s="4" t="n">
+      <c r="C100" s="5" t="n">
         <v>2000</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E100" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F100" s="4" t="s">
+      <c r="F100" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G100" s="4" t="s">
+      <c r="G100" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H100" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I100" s="4" t="s">
+      <c r="H100" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I100" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J100" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K100" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L100" s="4" t="n">
+      <c r="J100" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K100" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L100" s="5" t="n">
         <v>453</v>
       </c>
-      <c r="M100" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N100" s="4" t="s">
+      <c r="M100" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N100" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="O100" s="6" t="s">
+      <c r="O100" s="9" t="s">
         <v>438</v>
       </c>
     </row>
@@ -33027,53 +33077,38 @@
         <v>442</v>
       </c>
     </row>
-    <row r="102" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="7" t="s">
+    <row r="102" s="14" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="14" t="s">
         <v>443</v>
       </c>
-      <c r="C102" s="7" t="n">
+      <c r="C102" s="14" t="n">
         <v>2018</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="D102" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="E102" s="7" t="s">
+      <c r="E102" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F102" s="7" t="s">
+      <c r="F102" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G102" s="7" t="s">
+      <c r="G102" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H102" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I102" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="J102" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K102" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L102" s="7" t="n">
+      <c r="H102" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I102" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="L102" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="M102" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="N102" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="O102" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH102" s="8" t="s">
+      <c r="AH102" s="15" t="s">
         <v>447</v>
       </c>
     </row>
@@ -33224,53 +33259,53 @@
         <v>461</v>
       </c>
     </row>
-    <row r="106" s="5" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="s">
+    <row r="106" s="14" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="C106" s="5" t="n">
+      <c r="C106" s="14" t="n">
         <v>2005</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="E106" s="5" t="s">
+      <c r="E106" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="F106" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="G106" s="5" t="s">
+      <c r="G106" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H106" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I106" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="J106" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K106" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L106" s="5" t="n">
+      <c r="H106" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I106" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J106" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K106" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L106" s="14" t="n">
         <v>172</v>
       </c>
-      <c r="M106" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="N106" s="5" t="s">
+      <c r="M106" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N106" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="O106" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH106" s="9" t="s">
+      <c r="O106" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH106" s="15" t="s">
         <v>466</v>
       </c>
     </row>
@@ -33509,200 +33544,200 @@
         <v>487</v>
       </c>
     </row>
-    <row r="112" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="4" t="s">
+    <row r="112" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="C112" s="4" t="n">
+      <c r="C112" s="5" t="n">
         <v>2011</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="E112" s="4" t="s">
+      <c r="E112" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F112" s="4" t="s">
+      <c r="F112" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G112" s="4" t="s">
+      <c r="G112" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H112" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I112" s="4" t="s">
+      <c r="H112" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I112" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J112" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K112" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L112" s="4" t="n">
+      <c r="J112" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K112" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L112" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="M112" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N112" s="4" t="s">
+      <c r="M112" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N112" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="O112" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH112" s="4" t="s">
+      <c r="O112" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH112" s="5" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="113" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="4" t="s">
+    <row r="113" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="C113" s="4" t="n">
+      <c r="C113" s="5" t="n">
         <v>2011</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E113" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F113" s="4" t="s">
+      <c r="F113" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G113" s="4" t="s">
+      <c r="G113" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H113" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I113" s="4" t="s">
+      <c r="H113" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I113" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J113" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K113" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L113" s="4" t="n">
+      <c r="J113" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K113" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L113" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="M113" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N113" s="4" t="s">
+      <c r="M113" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N113" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="O113" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="114" s="4" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="4" t="s">
+      <c r="O113" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="114" s="10" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="C114" s="4" t="n">
+      <c r="C114" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E114" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F114" s="4" t="s">
+      <c r="F114" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="G114" s="4" t="s">
+      <c r="G114" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H114" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I114" s="4" t="s">
+      <c r="H114" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I114" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J114" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K114" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L114" s="4" t="n">
+      <c r="J114" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K114" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L114" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="M114" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N114" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="O114" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="AH114" s="4" t="s">
+      <c r="M114" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N114" s="13" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O114" s="10" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AH114" s="10" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="115" s="5" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="s">
+    <row r="115" s="14" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="14" t="s">
         <v>496</v>
       </c>
-      <c r="C115" s="5" t="n">
+      <c r="C115" s="14" t="n">
         <v>2018</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="E115" s="5" t="s">
+      <c r="E115" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F115" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="G115" s="5" t="s">
+      <c r="G115" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H115" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I115" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J115" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K115" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L115" s="5" t="n">
+      <c r="H115" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I115" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J115" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K115" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L115" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="M115" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="N115" s="5" t="s">
+      <c r="M115" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N115" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="O115" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH115" s="9" t="s">
+      <c r="O115" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH115" s="15" t="s">
         <v>499</v>
       </c>
     </row>
@@ -33835,341 +33870,341 @@
         <v>511</v>
       </c>
     </row>
-    <row r="119" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="4" t="s">
+    <row r="119" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="C119" s="4" t="n">
+      <c r="C119" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="E119" s="4" t="s">
+      <c r="E119" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F119" s="4" t="s">
+      <c r="F119" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="G119" s="4" t="s">
+      <c r="G119" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H119" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I119" s="4" t="s">
+      <c r="H119" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I119" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J119" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K119" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L119" s="4" t="n">
+      <c r="J119" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K119" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L119" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="M119" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N119" s="4" t="s">
+      <c r="M119" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N119" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="O119" s="4" t="s">
+      <c r="O119" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="P119" s="4" t="s">
+      <c r="P119" s="10" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="120" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="4" t="s">
+    <row r="120" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="C120" s="4" t="n">
+      <c r="C120" s="5" t="n">
         <v>2012</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="E120" s="4" t="s">
+      <c r="E120" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="F120" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="G120" s="4" t="s">
+      <c r="G120" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H120" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I120" s="4" t="s">
+      <c r="H120" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I120" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J120" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K120" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L120" s="4" t="n">
+      <c r="J120" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K120" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L120" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M120" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N120" s="4" t="s">
+      <c r="M120" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N120" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="O120" s="4" t="s">
+      <c r="O120" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="P120" s="4" t="s">
+      <c r="P120" s="5" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="121" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4" t="s">
+    <row r="121" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="C121" s="4" t="n">
+      <c r="C121" s="5" t="n">
         <v>2012</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E121" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="F121" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="G121" s="4" t="s">
+      <c r="G121" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H121" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I121" s="4" t="s">
+      <c r="H121" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I121" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J121" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K121" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L121" s="4" t="n">
+      <c r="J121" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K121" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L121" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M121" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N121" s="4" t="s">
+      <c r="M121" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N121" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="O121" s="4" t="s">
+      <c r="O121" s="5" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="122" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="4" t="s">
+    <row r="122" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="C122" s="4" t="n">
+      <c r="C122" s="5" t="n">
         <v>2002</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="E122" s="4" t="s">
+      <c r="E122" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F122" s="4" t="s">
+      <c r="F122" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="G122" s="4" t="s">
+      <c r="G122" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H122" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I122" s="4" t="s">
+      <c r="H122" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I122" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J122" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K122" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L122" s="4" t="n">
+      <c r="J122" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K122" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L122" s="5" t="n">
         <v>175</v>
       </c>
-      <c r="M122" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N122" s="4" t="s">
+      <c r="M122" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N122" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="O122" s="4" t="s">
+      <c r="O122" s="5" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="123" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4" t="s">
+    <row r="123" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="C123" s="4" t="n">
+      <c r="C123" s="5" t="n">
         <v>2002</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D123" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="E123" s="4" t="s">
+      <c r="E123" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F123" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="G123" s="4" t="s">
+      <c r="G123" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H123" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I123" s="4" t="s">
+      <c r="H123" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I123" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J123" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K123" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L123" s="4" t="n">
+      <c r="J123" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K123" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L123" s="5" t="n">
         <v>175</v>
       </c>
-      <c r="M123" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N123" s="4" t="s">
+      <c r="M123" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N123" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="O123" s="4" t="s">
+      <c r="O123" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="P123" s="4" t="s">
+      <c r="P123" s="5" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="4" t="s">
+    <row r="124" s="10" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="C124" s="4" t="n">
+      <c r="C124" s="10" t="n">
         <v>2002</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D124" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="E124" s="4" t="s">
+      <c r="E124" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F124" s="4" t="s">
+      <c r="F124" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="G124" s="4" t="s">
+      <c r="G124" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H124" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I124" s="4" t="s">
+      <c r="H124" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I124" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J124" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K124" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L124" s="4" t="n">
+      <c r="J124" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K124" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L124" s="10" t="n">
         <v>175</v>
       </c>
-      <c r="M124" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N124" s="6" t="s">
+      <c r="M124" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N124" s="13" t="s">
         <v>526</v>
       </c>
-      <c r="O124" s="6" t="s">
+      <c r="O124" s="13" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="125" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="5" t="s">
+    <row r="125" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="14" t="s">
         <v>528</v>
       </c>
-      <c r="C125" s="5" t="n">
+      <c r="C125" s="14" t="n">
         <v>2010</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="E125" s="5" t="s">
+      <c r="E125" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="F125" s="5" t="s">
+      <c r="F125" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="G125" s="5" t="s">
+      <c r="G125" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H125" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I125" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J125" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K125" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L125" s="5" t="n">
+      <c r="H125" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I125" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J125" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K125" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L125" s="14" t="n">
         <v>39</v>
       </c>
-      <c r="M125" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="N125" s="5" t="s">
+      <c r="M125" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N125" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="O125" s="5" t="s">
+      <c r="O125" s="14" t="s">
         <v>291</v>
       </c>
     </row>
@@ -34251,110 +34286,104 @@
       <c r="I127" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="J127" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K127" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="L127" s="0" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="128" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="4" t="s">
+    <row r="128" s="10" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A128" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="C128" s="4" t="n">
+      <c r="C128" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E128" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F128" s="4" t="s">
+      <c r="F128" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G128" s="4" t="s">
+      <c r="G128" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H128" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I128" s="4" t="s">
+      <c r="H128" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I128" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J128" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K128" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L128" s="4" t="n">
+      <c r="J128" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K128" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L128" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="M128" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N128" s="4" t="s">
+      <c r="M128" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N128" s="10" t="s">
         <v>540</v>
       </c>
-      <c r="O128" s="6" t="s">
+      <c r="O128" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="AH128" s="6" t="s">
+      <c r="AH128" s="13" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="129" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="4" t="s">
+    <row r="129" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A129" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="C129" s="4" t="n">
+      <c r="C129" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E129" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F129" s="4" t="s">
+      <c r="F129" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="G129" s="4" t="s">
+      <c r="G129" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H129" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I129" s="4" t="s">
+      <c r="H129" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I129" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J129" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K129" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L129" s="4" t="n">
+      <c r="J129" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K129" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L129" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M129" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N129" s="6" t="s">
+      <c r="M129" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N129" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="O129" s="6" t="s">
+      <c r="O129" s="9" t="s">
         <v>544</v>
       </c>
     </row>
@@ -34552,53 +34581,53 @@
         <v>291</v>
       </c>
     </row>
-    <row r="134" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="5" t="s">
+    <row r="134" s="14" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A134" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="C134" s="5" t="n">
+      <c r="C134" s="14" t="n">
         <v>2003</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="14" t="s">
         <v>565</v>
       </c>
-      <c r="E134" s="5" t="s">
+      <c r="E134" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="F134" s="5" t="s">
+      <c r="F134" s="14" t="s">
         <v>566</v>
       </c>
-      <c r="G134" s="5" t="s">
+      <c r="G134" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H134" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I134" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J134" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K134" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L134" s="5" t="n">
+      <c r="H134" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I134" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J134" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K134" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L134" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="M134" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="N134" s="5" t="s">
+      <c r="M134" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N134" s="14" t="s">
         <v>567</v>
       </c>
-      <c r="O134" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH134" s="9" t="s">
+      <c r="O134" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH134" s="15" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34649,144 +34678,144 @@
         <v>572</v>
       </c>
     </row>
-    <row r="136" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="4" t="s">
+    <row r="136" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="C136" s="4" t="n">
+      <c r="C136" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="E136" s="4" t="s">
+      <c r="E136" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F136" s="4" t="s">
+      <c r="F136" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="G136" s="4" t="s">
+      <c r="G136" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H136" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I136" s="4" t="s">
+      <c r="H136" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I136" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J136" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K136" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L136" s="4" t="n">
+      <c r="J136" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K136" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L136" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="M136" s="4" t="s">
+      <c r="M136" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="N136" s="4" t="s">
+      <c r="N136" s="10" t="s">
         <v>576</v>
       </c>
-      <c r="O136" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="137" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="4" t="s">
+      <c r="O136" s="10" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="137" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="C137" s="4" t="n">
+      <c r="C137" s="5" t="n">
         <v>2013</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="E137" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F137" s="4" t="s">
+      <c r="F137" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="G137" s="4" t="s">
+      <c r="G137" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H137" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I137" s="4" t="s">
+      <c r="H137" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I137" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J137" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K137" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L137" s="4" t="n">
+      <c r="J137" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K137" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L137" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="M137" s="4" t="s">
+      <c r="M137" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="N137" s="4" t="s">
+      <c r="N137" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="O137" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="138" s="4" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="4" t="s">
+      <c r="O137" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="138" s="5" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A138" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="C138" s="4" t="n">
+      <c r="C138" s="5" t="n">
         <v>2013</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F138" s="4" t="s">
+      <c r="F138" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="G138" s="4" t="s">
+      <c r="G138" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H138" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I138" s="4" t="s">
+      <c r="H138" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I138" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J138" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K138" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L138" s="4" t="n">
+      <c r="J138" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K138" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L138" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="M138" s="6" t="s">
+      <c r="M138" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="N138" s="6" t="s">
+      <c r="N138" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="O138" s="4" t="s">
+      <c r="O138" s="5" t="s">
         <v>582</v>
       </c>
     </row>
@@ -34951,51 +34980,51 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" s="7" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="7" t="s">
+    <row r="143" s="14" customFormat="true" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A143" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B143" s="14" t="s">
         <v>597</v>
       </c>
-      <c r="C143" s="7" t="n">
+      <c r="C143" s="14" t="n">
         <v>2018</v>
       </c>
-      <c r="D143" s="7" t="s">
+      <c r="D143" s="14" t="s">
         <v>598</v>
       </c>
-      <c r="E143" s="7" t="s">
+      <c r="E143" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F143" s="7" t="s">
+      <c r="F143" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="G143" s="7" t="s">
+      <c r="G143" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H143" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I143" s="7" t="s">
+      <c r="H143" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I143" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="J143" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K143" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L143" s="7" t="n">
+      <c r="J143" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K143" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L143" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="M143" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="N143" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="O143" s="8" t="s">
-        <v>599</v>
+      <c r="M143" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="N143" s="14" t="s">
+        <v>1128</v>
+      </c>
+      <c r="O143" s="15" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35301,144 +35330,144 @@
         <v>628</v>
       </c>
     </row>
-    <row r="150" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="4" t="s">
+    <row r="150" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="C150" s="4" t="n">
+      <c r="C150" s="5" t="n">
         <v>2018</v>
       </c>
-      <c r="D150" s="4" t="s">
+      <c r="D150" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="E150" s="4" t="s">
+      <c r="E150" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F150" s="4" t="s">
+      <c r="F150" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G150" s="4" t="s">
+      <c r="G150" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H150" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I150" s="4" t="s">
+      <c r="H150" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I150" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J150" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K150" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L150" s="4" t="n">
+      <c r="J150" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K150" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L150" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M150" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N150" s="4" t="s">
+      <c r="M150" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N150" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="O150" s="4" t="s">
+      <c r="O150" s="5" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="151" s="4" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="4" t="s">
+    <row r="151" s="5" customFormat="true" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A151" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="C151" s="4" t="n">
+      <c r="C151" s="5" t="n">
         <v>2018</v>
       </c>
-      <c r="D151" s="4" t="s">
+      <c r="D151" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="E151" s="4" t="s">
+      <c r="E151" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F151" s="4" t="s">
+      <c r="F151" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G151" s="4" t="s">
+      <c r="G151" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H151" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I151" s="4" t="s">
+      <c r="H151" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I151" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J151" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K151" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L151" s="4" t="n">
+      <c r="J151" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K151" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L151" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M151" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N151" s="6" t="s">
+      <c r="M151" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="N151" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="O151" s="4" t="s">
+      <c r="O151" s="5" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="152" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="4" t="s">
+    <row r="152" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="C152" s="4" t="n">
+      <c r="C152" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="D152" s="4" t="s">
+      <c r="D152" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="E152" s="4" t="s">
+      <c r="E152" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="F152" s="4" t="s">
+      <c r="F152" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="G152" s="4" t="s">
+      <c r="G152" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H152" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I152" s="4" t="s">
+      <c r="H152" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I152" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="J152" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K152" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L152" s="4" t="n">
+      <c r="J152" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K152" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L152" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M152" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="N152" s="4" t="s">
+      <c r="M152" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N152" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="O152" s="4" t="s">
+      <c r="O152" s="10" t="s">
         <v>291</v>
       </c>
     </row>
@@ -35574,90 +35603,90 @@
         <v>652</v>
       </c>
     </row>
-    <row r="156" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="4" t="s">
+    <row r="156" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="C156" s="4" t="n">
+      <c r="C156" s="5" t="n">
         <v>2011</v>
       </c>
-      <c r="D156" s="4" t="s">
+      <c r="D156" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="E156" s="4" t="s">
+      <c r="E156" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="F156" s="4" t="s">
+      <c r="F156" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="G156" s="4" t="s">
+      <c r="G156" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H156" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I156" s="4" t="s">
+      <c r="H156" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I156" s="5" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="157" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="4" t="s">
+    <row r="157" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="10" t="s">
         <v>653</v>
       </c>
-      <c r="C157" s="4" t="n">
+      <c r="C157" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="D157" s="4" t="s">
+      <c r="D157" s="10" t="s">
         <v>654</v>
       </c>
-      <c r="E157" s="4" t="s">
+      <c r="E157" s="10" t="s">
         <v>649</v>
       </c>
-      <c r="F157" s="4" t="s">
+      <c r="F157" s="10" t="s">
         <v>655</v>
       </c>
-      <c r="G157" s="4" t="s">
+      <c r="G157" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H157" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I157" s="4" t="s">
+      <c r="H157" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I157" s="10" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="158" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="4" t="s">
+    <row r="158" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="C158" s="4" t="n">
+      <c r="C158" s="5" t="n">
         <v>2011</v>
       </c>
-      <c r="D158" s="4" t="s">
+      <c r="D158" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="E158" s="4" t="s">
+      <c r="E158" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="F158" s="4" t="s">
+      <c r="F158" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="G158" s="4" t="s">
+      <c r="G158" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H158" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I158" s="4" t="s">
+      <c r="H158" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I158" s="5" t="s">
         <v>356</v>
       </c>
     </row>
@@ -38726,7 +38755,7 @@
       <c r="M221" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="N221" s="10" t="s">
+      <c r="N221" s="2" t="s">
         <v>356</v>
       </c>
       <c r="O221" s="0" t="s">
@@ -40943,7 +40972,7 @@
   </sheetPr>
   <dimension ref="A1:AH263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>

</xml_diff>

<commit_message>
Began coding operationalizations (ended at line 86); split codes into separate spreadsheet; updated coding rules
</commit_message>
<xml_diff>
--- a/ses_scoreBox_compiled3-FOR CODING.xlsx
+++ b/ses_scoreBox_compiled3-FOR CODING.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12821" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12821" uniqueCount="1142">
   <si>
     <t xml:space="preserve">reviewer</t>
   </si>
@@ -615,12 +615,9 @@
   </si>
   <si>
     <t xml:space="preserve">It is measured using the three indicators of SES available in the TDCRP database: the ISP, education, and family income. p.151
-How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005
-_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [education]). Predetermined cutoff scores then assign individuals to one of five social classes. In all analyses, the ISP was used as a categorical variable, with patients in Classes II and III (middleclass patients) as the reference group, and comparing both patients in Class I (upper class) and in Classes IV 
-nd V (working class and poor) to those in Classes II and III". p.151
-How education was measured: In all analyses, education was used as a categorical variable, comparing patients with a high school diploma or less education with patients who had completed more education than a high school diploma.p.151
-Haven't seen how income was meausred. 
-</t>
+How ISP was measured: "The Hollingshead Two-Factor ISP (Hollingshead, 1971) uses a combination of education and occupation ratings to categorize individuals into five social classes, which correspond roughly with upper class (Class I), the middle classes (Classes II and III), the working class (Class IV), and the poor (Class V). An individual’s education level is rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ completed graduate or professional training to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ under seven years of schooling. Occupational prestige is also rated on a 7-point scale, from 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ higher executives, proprietors of large concerns, and major professionals to 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_
+005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ unskilled employees. These two ratings are then combined as follows: (7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005
+_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ [occupation]) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ (4 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x</t>
   </si>
   <si>
     <t xml:space="preserve">The reason for why using ISP, family income and education as indicators: "These three indicators are the most commonly used indicators of SES in psychotherapy research (Garfield, 1994) and allow for comparison with this literature. In particular, Liu et al. (2004) found, in their review of empirical research articles that included SES, that the ISP was the most commonly used measure of SES. In this study, using all three indicators serves the purpose of attempting to address discrepancies in the literature on SES and treatment outcome, because most studies have used only one of these three indicators, with varying results". p.151
@@ -701,7 +698,7 @@
     <t xml:space="preserve">Yes(IV)</t>
   </si>
   <si>
-    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
+    <t xml:space="preserve">The occupational prestige level was coded using Duncan’s Socioeconomic Index (Mueller &amp; Parcel, 1981) and was similar across ethnic groups for mothers. However, African American fathers were employed in positions with lower prestige than were Euro-American fathers, F(1, 73) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.78, p .05. Chi-square statistics were used to assess ethnic differences in categorical demographic data. Across ethnic groups, parents were similar in employment status (i.e., being unemployed or employed part time or full time) and family income levels, according to chi-square analysis. There were equal numbers of African American and Euro-American families above and below the state median family income (i.e., $32,000; U.S. Census Bureau, 1999). Annual family income levels ranged from less than $5,000 to above $90,000, with a mean range between $32,001 and $39,000. Neither were there ethnic differences in the number of families receiving Aid for Families with Dependent Children or supplemental security income supplements to their family income.(pg.211)</t>
   </si>
   <si>
     <t xml:space="preserve">Because many studies that have examined these relationships among African American and Euro-American families have confounded ethnicity with socioeconomic status, we included African American and Euro-American families from comparable but diverse socioeconomic backgrounds.(pg.210) Because socioeconomic status and ethnicity are often confounded in studies of ethnic minority and majority populations and
@@ -788,7 +785,7 @@
     <t xml:space="preserve"> 3211 Affective Disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
+    <t xml:space="preserve">An SES scale was created by combining information on occupation, education, and income and was based on the Hollingshead scale (Hollingshead, 1975). We created a modiﬁed scale because of a lack of detailed information on occupation in our survey. Scores ranged from 0 to 6, with a higher score suggesting more favorable or higher SES. The three variables were summed to form the following categories: (a) occupation: professional (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), skilled laborer (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), unskilled laborer (0); (b) income: more than $50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), $25K–$50K (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), under $25K (0); and (c) education: more than high school (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2), high school or GED (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1), less than high school (0). Other SES measures in our model included participants’ satisfaction with their current ﬁnancial situation, poverty income ratio, and type of health insurance. p.5</t>
   </si>
   <si>
     <t xml:space="preserve">I am not sure about the mainEffect. Low SES will increase the level of anxiety, stress, and  through which it will increase the rate of depression. SES seems to be a background factor instead of direct cause in the study. 
@@ -948,7 +945,7 @@
     <t xml:space="preserve">None given</t>
   </si>
   <si>
-    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
+    <t xml:space="preserve">We created separate composite variables at T1, T2, and T3 from family income and mother and father education. Maternal reports of total family income were gathered and classified into one of the following categories: (a) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_10,000; (b) $10,000 to $20,000; (c) $20,000 to $35,000; (d) $35,000 to $50,000; (e) $50,000 to $75,000; or (f) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_$75,000. Mother’s and father’s years of education were also gathered. Following the recommendations of Braveman and colleagues (2005), the indicators were standardized and then summed to create separate composite variables representing overall SES at T1, T2, and T3. p.1507</t>
   </si>
   <si>
     <t xml:space="preserve">Why not mainEffect? SES serves as a moderator, as seen in "socioeconomic status (SES; controlling for ethnicity) and ethnicity (controlling for SES) moderated the relation between sleep and cognitive performance". 
@@ -1026,7 +1023,7 @@
     <t xml:space="preserve">3550 Academic Learning &amp; Achievement</t>
   </si>
   <si>
-    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
+    <t xml:space="preserve">As noted earlier, parent education and family income served as measures of SES. Because parent education and family income were moderately related to one another (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .48, p .01), we combined them into one variable of SES using principal components analysis. The first principle component weighted education and income positively and equally and accounted for 74% of the original variance. The mean score of the composite was 0 (SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1). Families that scored high on the SES composite had high annual income levels and the primary caregiver had a high level of education. (pg.1313)</t>
   </si>
   <si>
     <t xml:space="preserve">Used principal component analysis</t>
@@ -1048,7 +1045,7 @@
   </si>
   <si>
     <t xml:space="preserve">Why IV and mainEffect? &gt; SES was tested independently, as suggest in "Although SES and other noninjury variables are known to affect outcomes of children with TBI (Taylor, 2004; Taylor et al., 1999, 2002; Yeates et al., 1997), no significant effect of SES on event-based PM performance was found". P.206 
-SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
+SA: Great calls. See also: “ Other main effectsevaluated included Age-at-Test, Gender, Socioeconomic Status(SES; estimated by the mother’s education level), Group, Motiva-tion Condition, and the Group_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_Motivation Condition interaction.” (p. 204)</t>
   </si>
   <si>
     <t xml:space="preserve">Nicholls, Michael E. R.;Johnston, David W.;Shields, Michael A.</t>
@@ -1613,7 +1610,7 @@
     <t xml:space="preserve">"Initial studies investigating vocabulary growth focused on the quantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)found that the most striking differences in input were in amount rather than richness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-class families were exposed to 25 past tenses per hour, and those on welfare families only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed to more varied vocabulary improved more quickly (Hoff, 2003), and that this influence could be independent of the quantity of child-directed speech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntactic diversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement the transform on the past-tense input as a modulation of the type frequency of verbs." (p. 2331)</t>
   </si>
   <si>
-    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
+    <t xml:space="preserve">This was a complicated paper. MainEffect should be yes becaus the authors want to know how SES affects acquisition of the past tense. The authors really did only one study, the simulation. So, we should use the operationalization's and justifications for that study. Here is what I'd put for the operationalization: "On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs. A lower SES family would be modeled asusing fewer past tenses overall, fewer types of regular verbs, andfewer types of irregular verbs. This implementation captures boththe reduced diversity of vocabulary in lower SES families and thereduced quantity of past tenses experienced by the child. In ma-chine learning terms, we operationalized environmental variationas a (potentially time-varying) function with respect to the trainingset. We assumed that there was a “perfect training set,” in this casecomprising all of the verbs available in the language, along with their accepted past-tense forms. We defined the function for vari-ations in the training set as follows:Training setPnTt_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_f_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_perfect training set,X,Y,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.(1)The training set for personnat timetis a functionfof the perfecttraining set and three parameters:X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of valid trainingtrials,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportion of invalid training trials, andZ_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_proportionof noise trials. Invalid trials have the same input as a trainingpattern but a different output. Noise trials have different inputs andoutputs or include partial information consistent with trainingpatterns. In principle, the functionfcould be influenced by personn’s behavior or experiences att_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_1, creating a more complexdynamical equation. A dynamical equation would accommodatethe possibility of, for instance, a reduced reward leading to reducedattention and therefore a subsequently smaller proportion of validtraining trials..... Todo so, we generated afamily quotientfor each simulated child.This was our implementation of SES. The family quotient was anumber between 0% and 100%. This value was used as a proba-bility determining whether each verb in the perfect training setwould be included in the family’s vocabulary. In terms of Equation1,X_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_family quotient,Y_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0,Z_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_0. The family training set wasthen fixed throughout development. However, performance wasalways assessed against the full perfect training set (analogous toa standardized test of past-tense formation applied to all children).The family quotient manipulation corresponds to a reduction intype frequency for both regular and irregular verbs, while the tokenfrequency of each verb (3 times greater presentation for high thanlow frequency) was retained.Our final decision was how to sample the family quotientvalues. The composite SES measure used for theBishop (2005)sample of twins had a normal distribution with large standarddeviation and a negative skew. Another twin study examining SESeffects on cognition with a large sample of 287 school-age children(Hart et al., 2007) reported maternal education data that werenormally distributed with a large standard deviation and a positiveskew. In the end, we selected a uniform distribution, which slightlyexaggerated the incidence of high and low SES. We selected tworanges of environmental variation: a narrow range with reasonablyhigh quality, sampling family quotient values between 60% and100%, and a wide range that accommodated potentially very poorquality environments, sampling quotient values between 0% and100%. These manipulations were applied equally to regular andirregular verbs." (p. 2331). For reason, I would put "Initial studies investigating vocabulary growth focused on thequantity of language to which children are exposed (Hoff-Ginsberg,1991,1992;Huttenlocher, Haight, Bryk, Seltzer, &amp; Lyons, 1991).Across a range of language features,Hart and Risley (1995)foundthat the most striking differences in input were in amount rather thanrichness (e.g., children in professional families were exposed to 36past tenses per hour on average, whereas those in working-classfamilies were exposed to 25 past tenses per hour, and those in welfarefamilies only 8 per hour; p. 243, Figure 11). Nevertheless,Hart andRisley (1992)reported that in general parents who used more wordstended to use a greater variety of words and in longer sentences.Studies of vocabulary growth have indicated that children exposed tomore varied vocabulary improved more quickly (Hoff, 2003), and thatthis influence could be independent of the quantity of child-directedspeech (Huttenlocher et al., 2010;Pan, Rowe, Singer, &amp; Snow, 2005).Huttenlocher et al. (2010)found that this effect also held for syntacticdiversity, while quantity influenced the order of emergence of struc-tures within a child.On the basis of this literature, we chose to implement thetransform on the past-tense input as a modulation of the typefrequency of verbs." (p. 2331)</t>
   </si>
   <si>
     <t xml:space="preserve">Tsethlikai, Monica</t>
@@ -1665,11 +1662,11 @@
     <t xml:space="preserve">Early temperamental and family predictors of shyness and anxiety</t>
   </si>
   <si>
-    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
+    <t xml:space="preserve">We measured families’ SES with a modified version of Hollingshead’s (1957) index on three occasions: study entry (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 48.77, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.611, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 242), 30 months (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.67, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 10.167, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 120), and 7 years of age (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 49.40, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 8.75, n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 172). Hollingshead’s index takes into account caregivers’ levels of education and current occupations (pg.1196).Average SES. The scores computed using an updated version
 of Hollingshead’s (1957) index were based on parents’ education
 levels and occupations. Because the scores measured at study
 entry, 30 months, and the 7– 8 years of age follow-up were highly
-correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
+correlated (range _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .68 –.74), they were averaged into one overall
 SES score (pg. 1198).</t>
   </si>
   <si>
@@ -1746,26 +1743,26 @@
     <t xml:space="preserve">"The relatively stable contex- tual factors of family-of-origin SES (education and occupation) and income were tested because they were hypothesized to relate to ongoing developmental contextual risk for the youth." (p. 395)</t>
   </si>
   <si>
-    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
+    <t xml:space="preserve">"Family income was the mean of both parents’ reports and was coded in eight categories: The first six consisted of the $5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and 8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_. Family income was calculated for Study Years 3, 7, and 9.Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index".Again, SES was scored for Study Years 3, 5, and 7. p.397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family income and SES were significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ .01) and therefore were combined by taking the mean of their standardized scores to arrive at a global measure of SES/income over Study Years 3, 5, and 7. p.397 </t>
   </si>
   <si>
     <t xml:space="preserve">Family income was the mean of both parents’
 reports and was coded in eight categories: The first six consisted of the
-$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
-8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
+$5,000 increments from 0 through $29,999, 7 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $30,000–$39,999, and
+8 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ $40,000. Family income was calculated for Study Years 3, 7, and 9.
 Parents’ occupations and educational levels were classified and combined according to the Hollingshead (1975) four-factor index. Again, SES
 was scored for Study Years 3, 5, and 7. Family income and SES were
-significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
+significantly associated (r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .41, p  .01) and therefore were combined by
 taking the mean of their standardized scores to arrive at a global measure
 of SES/income over Study Years 3, 5, and 7. (pg. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">The relatively stable contextual factors of family-of-origin SES (education and occupation)
 and income were tested because they were hypothesized to relate
-to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
+to ongoing developmental contextual risk for the youth.  (pg. 395) “Family  income  and  SES  weresignificantly associated (r_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_.41,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.01) and therefore were combined bytaking the mean of their standardized scores to arrive at a global measureof SES/income over Study Years 3, 5, and 7.” (p. 397)</t>
   </si>
   <si>
     <t xml:space="preserve">Corley, Janie;Gow, Alan J.;Starr, John M.;Deary, Ian J.</t>
@@ -1882,7 +1879,7 @@
 year. Two of the three questions were on a five-point Likert-type
 scale; the third was on a four-point scale. Standardized scores were
 generated for this scale and higher scores were representative of
-less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
+less economic pressure;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .82 in the current sample. The second
 indicator (material needs) comprised seven questions assessing
 how mothers felt about their family’s economic situation (e.g.,
 “My family has enough money to afford the kind of home we
@@ -1891,12 +1888,12 @@
 (Conger et al., 1992), lower scores indicate less material needs and
 more economic well-being; however, we reversed the score to
 make it compatible with the others and thus in all analyses higher
-scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
+scores represent more economic well-being ( _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .92). The final
 economic well-being indicator (financial cutbacks) comprised 22
 statements describing adjustments the family had to make over the
 last year because of financial need (e.g., using savings to meet
 daily living expenses). Higher scores were indicative of a better
-economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
+economic situation;  _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .86 (pg. 851-852).</t>
   </si>
   <si>
     <t xml:space="preserve">"The operational definition of SES has long been debated be-
@@ -1921,7 +1918,7 @@
 Mplus and showed excellent measurement properties. The three
 observed measures— can’t make ends meet, material needs, and
 financial cutbacks—loaded well on the latent variable of perceived
-economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
+economic well-being (r values _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .76 to .87); all were coded and
 analyzed such that higher levels are indicative of a better economic
 situation" (pg. 853)"For reason for operationalization, I think the following is sufficient: "The operational definition of SES has long been debated be-
 cause of its multidimensional nature (for review see Hout, 2008).
@@ -1956,9 +1953,9 @@
 linked to obesity than family income (Shrewsbury &amp; Wardle,
 2008). Seven response options were provided to report the highest
 education completed ( eighth grade, some high school, high
-school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
+school graduate, GED [general equivalence diploma], some college, 4-year college degree, _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_4-year college degree), some of
 which were combined to reduce categories with small prevalence
-such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
+such that four SES strata were differentiated in the analysis: _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005_
 high school graduate, high school graduate (including GED), some
 college, and 4-year college degree household. (pg. 3)</t>
   </si>
@@ -1991,7 +1988,7 @@
   </si>
   <si>
     <t xml:space="preserve">It seems like SES was used only as a control. 
-Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
+Great job on this study. I have no idea why the authors reported the correlation with SES. The only quote I found on operationalizing SES was in the Note for Table 2: “; SES_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ = socioeconomic status (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=low, 2=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_normal, 3=_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high)” (p. 374), which is utterly uninformative but we should include anyway.  &gt; adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Kiviniemi, Marc T.;Klasko-Foster, Lynne B.;Erwin, Deborah O.;Jandorf, Lina</t>
@@ -2047,8 +2044,9 @@
 10-rung ladder representing society, with those at the top (bottom)
 of the ladder being the best (worst) off and having the most (least)
 education, money, and best (worst) jobs. Higher scores on the
-10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
-1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
+10-rung ladder indicated higher subjective SES (M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 5.35, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_
+1.86). (pg.139) .  Objective SES was assessed using selfreports of educational attainment and annual income.  (pg.139) education and income: Educationwas assessed using four categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_did not finish high school,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_high school graduation,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_college graduation,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_post-graduate degree;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_2.73,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_0.72). Annual income wasassessed using eight categories (1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_less than $15,000,2_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$15,001–25,000,3_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$25,001–35,000,4_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$35,001–50,000,5_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$50,001–75,000,6_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$75,001–100,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0
+5F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_$100,001–150,000,8_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_greater than $150,000;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_4.29,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_1.90)” (p. 140)</t>
   </si>
   <si>
     <t xml:space="preserve">‘“However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood.” (p. 138)</t>
@@ -2163,7 +2161,7 @@
     <t xml:space="preserve"> 2800 Developmental Psychology , 2500 Physiological Psychology &amp; Neuroscience</t>
   </si>
   <si>
-    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
+    <t xml:space="preserve">We quantified socioeconomic risk exposure using a cumulative approach with discrete, additive markers. Consistent with previous studies using the cumulative risk framework, we examined single parenthood, low maternal education, and low household income as the primary socioeconomic risk factors (e.g., Evans, 2003; Evans &amp; Kim, 2010). For each of the three indicators, risk was coded dichotomously as present (1) or not present (0), with each risk factor aimed to characterize the riskiest third of the sample for that dimension. Household income risk was quantified as households in the bottom third of annual income to needs ratio within the sample, here households with income to needs ratios less than 0.5 (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 33). Income to needs ratios were calculated from self-reported income and number of people supported by the income, based on the 2017 federal poverty guidelines from the Department of Health and Human Services (https://aspe.hhs.gov/poverty-guidelines). Maternal education risk was quantified as households in which the mother’s highest degree of education was a high school diploma or less (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 39). Marital status risk was quantified as single parent households, in this case all single mothers (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 32). p.1676 -1677</t>
   </si>
   <si>
     <t xml:space="preserve">Why MainInterest &gt; In the current study, we test two main hypotheses related to early adversity. First, we hypothesized that exposure to a greater number of socioeconomic risk factors, such as low household income, low maternal education, and single parent status (Evans, Li, &amp; Whipple, 2013), would be associated with differences in neural measures of children’s auditory selective attention, specifically distractor suppression (Stevens et al., 2009). Second, we hypothesized that socioeconomic risk would be associated with altered SNS and PNS function, with greater risk associated with heightened SNS activity, indexed by shorter PEP, and reduced PNS activity, indexed by lower baseline values of HF-HRV and reduced HF-HRV withdrawal to the task.
@@ -2222,7 +2220,7 @@
     <t xml:space="preserve">"Contextual SES factors such as literacy, education, occu- pation, income, and health status appear to be related to structural brain development and atrophy (Brito &amp; Noble, 2014; Farah et al., 2006; Fotenos, Mintun, Snyder, Morris, &amp; Buckner, 2008; Law- son, Duda, Avants, Wu, &amp; Farah, 2013; Raizada &amp; Kishiyama, 2010; Raz et al., 2005; Staff et al., 2012; Taki et al., 2011; Tomalski et al., 2013)." (p. 986)</t>
   </si>
   <si>
-    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
+    <t xml:space="preserve">The SES index was comprised of education and poverty status, with both variables dichotomized. Below median education (0 will be &gt;=12 years; 1 will be &lt; 12 years) and publishers income below 125% of the 2004 federal poverty line relative to family size and household income (0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ above the poverty line; 1  below the poverty line) was considered low SES. A composite score of SES was computed as a dichotomous variable, with low SES defined as below median education and/or income below 125% of the poverty line. Participants that met neither of those criteria were labeled as high SES.  p.997 -998
 Our SES measure also does not incorporate participants’ childhood SES, a variable that is especially important to consider when examining brain health (Staff et al., 2012). p. 992
 </t>
   </si>
@@ -2233,7 +2231,7 @@
     <t xml:space="preserve">2520 Neuropsychology &amp; Neurology</t>
   </si>
   <si>
-    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
+    <t xml:space="preserve">“The SES index was comprised ofeducation and poverty status, with both variables dichotomized.Below median education (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_=≥12 years; 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_=&lt;12 years) and income below 125% of the 2004 federal poverty line relative tofamily size and household income (0_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_above the poverty line;1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_below the poverty line) was considered low SES. A compositescore of SES was computed as a dichotomous variable, with lowSES defined as below median education and/or income below125% of the poverty line. Participants that met neither of thosecriteria were labeled as high SES.” (p. 987–988)</t>
   </si>
   <si>
     <t xml:space="preserve">Xing, Xiaopei;Wang, Meifang</t>
@@ -2279,7 +2277,7 @@
     <t xml:space="preserve">2260 Research Methods &amp; Experimental Design , 3000 Social Psychology</t>
   </si>
   <si>
-    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
+    <t xml:space="preserve">The average of the two parents’ Duncan Socioeconomic Index scores was used as the measure of SES (Stevens &amp; Featherman, 1981; M _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 40.83, SD _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 16.32).(pg.6)</t>
   </si>
   <si>
     <t xml:space="preserve">Great work! Only change is that MainInterest should be no. The authors included SES only as a control variable, and not even a particularly theoretically motivated one. Their main interest was just demonstrating how to model some data.</t>
@@ -2379,7 +2377,7 @@
     <t xml:space="preserve">Long-term outcome from childhood traumatic brain injury: Intellectual ability, personality, and quality of life</t>
   </si>
   <si>
-    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
+    <t xml:space="preserve">SES at time of injury was coded according to Daniel (1983) and based on highest occupational prestige of the participants’ parents, providing a 7-point rating with higher scores reﬂecting lower SES. These ratings were then categorized into High (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) or Low (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4) SES, as outlined in the rating manual. p.177</t>
   </si>
   <si>
     <t xml:space="preserve">This is a hard one for me. Why mainInterest = YES? Because "we hypothesized that noninjury indices, including SES and age factors, would play a significant role in determining intellect, personality, and QOL" p.181, even though the findings suggested that SES was not the main predictor. MainInterest should be determined by the hypothsis, not conclusion. 
@@ -2527,7 +2525,7 @@
     <t xml:space="preserve">Five different measures were used to represent low social status: income, education, gender, race/ethnicity, and social class. (P.769); 
 Participants’ family income was measured on a 5-point scale ranging from 1 (0 to 16th percentile) to 5 (96th percentile and above) in the ANES and a 10-point scale ranging from 1 ( lowest decile) to 10 ( highest decile) in the WVS.(P.770);  
 The income measure used in this study combines the different categorical income measures across the years and equates the different measures in terms of dollars in the year 2000 (for full details see Hout, 2004). P.770
-Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
+Race/ethnicity was coded as 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ ethnic minority (i.e., those not indicating “White”) and 1 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ White in the ANES and GSS. P.770
 Social class was measured with an 8-point scale ranging from 0 (lower class) to 7 (upper class) in the ANES; a 5-point scale ranging from 1 (lower class) to 5 (upper class) in the GSS; and a 5-point scale ranging from 1 (upper class) to 5 (lower class) in the WVS (reverse scored). All of the measures of social status were standardized to range from zero ( lowest status) to one ( highest status) to facilitate comparisons across measures and across samples. P.770</t>
   </si>
   <si>
@@ -2586,7 +2584,7 @@
     <t xml:space="preserve">Early adverse environments and genetic influences on age at first sex: Evidence for gene × environment interaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
+    <t xml:space="preserve">Socioeconomic status was measured using residential parent’s mean level of educational attainment. Educational attainment is a commonly used index of socioeconomic status (Bradley &amp; Corwyn, 2002), which might be more stable than family income (U.S. Treasury Department, 2008) and has been used in previous G _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ E analyses (e.g., Harden, Turkheimer, &amp; Loehlin, 2007). Educational attainment was coded on a 9-point ordinal scale ranging from eighth grade or less to professional training beyond a 4-year degree. p.1535</t>
   </si>
   <si>
     <t xml:space="preserve">Why mainInterest? "The goal of the current study was to test whether three broad markers of environmental risk—low socioeconomic status, biological father absence in childhood, and racial/ethnic minority status—moderate the heritability of AFS." p.1534
@@ -2628,7 +2626,7 @@
     <t xml:space="preserve">On the academic disadvantage of low social class individuals: Pursuing performance goals fosters the emergence of the achievement gap</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
+    <t xml:space="preserve">The relative social class manipulation was adapted from past research (see Adler et al., 2000; Kraus et al., 2010). The picture of a scale was described as representing people’s different social positions in France, and participants were required to imagine and write a few words about an interaction with either a high social class individual, who would stand at the very top of the ladder (low social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 90) or a low social class individual, who would stand at the very bottom of the ladder (high social class manipulation, N _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_ 86). In particular, they were instructed to think about how they differed from this category of people “who have the most [least] money, most [least] education, the most [least] respected jobs.” After they had written a few words about the imagined interaction, we asked participants to position themselves on that same ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 500 (top of the ladder). p.1264</t>
   </si>
   <si>
     <t xml:space="preserve">After having read and agreed to the consent form, participants were first introduced to the social class manipulation, which was identical to that used in Study 1. In the end of this manipulation, as in Study 1, we asked participants to position themselves on a ladder that symbolically represented the hierarchy of social class (Adler et al., 2000). They used a cursor, resulting in answers going from 0 (bottom of the ladder) to 9 (top of the ladder). p.1266</t>
@@ -2713,7 +2711,7 @@
     <t xml:space="preserve">Socioeconomic risk moderates the link between household chaos and maternal executive function</t>
   </si>
   <si>
-    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
+    <t xml:space="preserve">We computed a socioeconomic risk index by summing across five indicators. These were, in order from most to least frequent: single mother [1 (38% of sample), versus 0 = married or cohabiting with child’s father]; low paternal education [1 = high school/GED or less (30% of sample), versus 0 _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ some college or higher education]; housing [1 = apartment, townhouse, duplex, mobile home (26% of sample) versus 0 = separate single-family home]; low maternal education [1 = high school/GED or less (22% of sample), versus 0 = some college or higher education]; and paternal unemployment [1 =unemployed (18% of sample), versus 0 = employed]). These risk indicators all covaried, with Spearman rho coefficients ranging from .26 ( p =.01) to .44 (p = .001). The resulting distribution of the summed multiple-risk variable was: 0 risks (n = 64 or 41.8% of sample); 1 (n = 34, 22.2%); 2 (n =19, 12.4%); 3 (n = 19, 12.4%); 4 (n = 10, 6.5%); 5 (n = 7, 4.6%). Figure 1 shows the prevalence of each risk indicator as a function of overall multiple-risk status. There appeared to be fairly linear increases in the prevalence of each risk factor as a function of overall risk status, with the exception of father unemployment, which jumped from 10–21% for those with three or fewer risks to 80% for those with four risks. p.393</t>
   </si>
   <si>
     <t xml:space="preserve">We constructed a socioeconomic multiple risk variable from the sum of five socioeconomic risks.These included three commonly used risk factors: low mother education and low father education (i.e., a high school diploma or less), and father unemployment. As a fourth risk factor, we also included living in home that was not a detached single family house (i.e., apartment, townhouse, trailer/mobile home). This distinction in housing circumstances is associated with features of the ecology of the home and neighborhood that predict health and functioning, beyond measures of parental employment, income, and education (Diez–Roux et al., 2001). The fifth risk factor was single mother status, because it is the family structure attribute with the strongest links to family poverty and barriers to employment and education ( APA, 2007). p.392-393
@@ -3096,7 +3094,7 @@
 problem behaviors (Dodge, Pettit, &amp; Bates, 1994; Malti,
 Averdijk, Ribeaud, Rotenberg, &amp; Eisner, 2013). For example, both Turkish boys and girls with low SES have been
 shown to have higher reactive and proactive aggression
-scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
+scores than those with middle and high SES (Bas_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ &amp;
 Yurdabakan, 2012). Longitudinal studies even showed that
 low parental SES in childhood leads to higher mean levels
 of offspring anger and hostility when these were measured
@@ -3166,19 +3164,19 @@
     <t xml:space="preserve">“SES can be defined as a representation of an individual’s rela-tive position in an economic-social-cultural hierarchy tied topower, prestige, and control over resources (Weber, 1922)” (p. 1479)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_high school/GED, 21 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_PhD., MD, orother professional degree). Income and education were standard-ized and averaged to create a composite SES measure” (p. 1481) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">“Previous studies have differed widelyin the aspects of SES under investigation, mirroring the generaldiversity in approaches toward measuring SES (Diemer et al., 2013).Income and education are among the most widely studied aspectsof SES with substantial, but not high, intercorrelations (Ensminger,Fothergill, Bornstein, &amp; Bradley, 2003;Winkleby, Jatulis, Frank,&amp; Fortmann, 1992). Income captures a dynamic representation ofan individual’s access to and control over resources and can bequite variable from year to year (Duncan &amp; Rodgers, 1988);education (typically indexed by the highest education level com-pleted) is a more static SES measure.” (p. 1480)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
+    <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $0/lossto 31_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_$100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_no school/some grade school,12_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_greater than $150,000); and (b) highest completed years of edu-cation (i.e., “What is the highest level of education you haveobtained?;” 8 years_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0</t>
+    <t xml:space="preserve">“Socioeconomic status was measuredusing (a) household income (i.e., “What is your family’s annualhousehold income (before taxes)?;” 1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_less than $20,000,7_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x00</t>
   </si>
   <si>
     <t xml:space="preserve">“Socioeconomic status was measured atT1 and T2 using (a) income (i.e., T1: average of “What was yourpersonal income during the past 12 months?,” less than $0/loss to $100,000 or more; T2: The total income of the respondentduring the past 12 months summarizing “personal earning income,”“pension income,” and “social security income” was top-coded at$200,000; note that an identical item was not available at T1); and (b)education (i.e., “What is the highest grade of school or year of collegeyou completed?;” no school/some grade school, Ph.D,Ed.D, MD or other professional degree)…. A composite SES measure wascomputed from the standardized average for income and education” (p. 1483) [used items individually too]</t>
@@ -3306,7 +3304,7 @@
     <t xml:space="preserve">Psychology of Aesthetics, Creativity, and the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
+    <t xml:space="preserve">Parents’ educational level was an indicator of their socioeconomic status. A student’s mother’s and father’s educational level was coded on a four-point scale (1 – elementary, 2 – vocational, 3 – high school, 4 – college/university) and then summed. The reliability of this scale was satisfactory (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_ _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .73). p.157</t>
   </si>
   <si>
     <t xml:space="preserve">The author didn't explain why only education was used as an indicator. I suspect it's related to the proposed mechanism, "It was found that low SES parents concentrate on such uncreative child qualities as conformity, whereas higher SES parents support intellectual flexibility, nonconformity and imagination (Kohn &amp; Slomczynski, 2006)".  p.157</t>
@@ -3450,7 +3448,7 @@
   </si>
   <si>
     <t xml:space="preserve">used principal component factor analysis 
-SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
+SA: Pretty good job here. SES is a MainEffect because the authors want to know how scores on the three scales differ across SES. As for the operationalizations...it's complicated. The operationalization you noted in Study 1 is correct. We also need to note that the authors are using the samples themselves as proxies for SES (e.g., "The  online  sample  represented  much  higherSES  than  the  community  sample  (95%  com-pared  to  33%  with  a  college  education  and¥4,620  compared  to  ¥2,722  mean  income)." and " the differ-ence  between  the  two  samples  on  the  good-father  variable  was  the  highest  and  wassignificant  [Monline_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_Mcommunity_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.82,t(827)_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_15.55,p_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_.001]. These findings sup-port our hypothesis that contemporary women,especially those with high socioeconomic con-ditions,  value  good-father  attributes  morehighly than they value good-provider or good-genes  attributes  in  the  context  of  a  long-termrelationship." on p. 220–221 for S1; "we examined the effect of socio-economic  development  by  comparing  womenfrom  rural  villages  and  towns  in  which  eco-nomic development has been relatively behindor  delayed  with  women  from  urban  areas  ofChina" on p. 221 for S2). Also, the quotes for studies 2 and 3 are missing.</t>
   </si>
   <si>
     <t xml:space="preserve">Marsh, Herbert W.</t>
@@ -3620,7 +3618,7 @@
 Why mainInterest? &gt;&gt;&gt;"By comparing the supports children received across communities and contexts, we attempted to understand ... how home and school SES factors in neighborhoods may be inextricably connected".  p.103
 Wow this article was a doozy. Great job overall. From my read, it does seem like SES is main effect in this paper; the authors seem primarily interested in how students from the two communities they identified (which they call student-level SES) differ from each other. But then they also add Family SES (“ we added the individual family SES (acombi-nation of family income, education, and H.O.M.E scores) as a pre-dictive variable in the third step of the regression models.” p. 112). I have no idea what the authors did with the School SES variable you found the quote for. For operationalization, I would include the quote you have, and add the following:
 “In the present paper, we address this possible “double dose ofdisadvantage” by following a cluster sample of 70 children whohave recently made the transition from preschool to kindergarten.Thirty-five of the families and their children came from neighbor-hoods considered to reflect concentrated poverty (i.e., 40% ormore of residents identified as poor), while the remaining halfcame from contiguous “borderline” communities that are moredemographically diverse and largely working-class...in which the poverty rate generally rangesfrom 20–40%.” (p. 103–104)
-“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
+“Home observation for the measurement of the environment.During the first home visit, trained research assistants administeredthe Home Observation for the Measurement of the Environment(H.O.M.E.;Bradley, Caldwell, &amp; Corwyn, 2003), a widely usedobservational measure designed to examine the quality and quan-tity of cognitive stimulation and material support in children’shomes. H.O.M.E. has been used extensively in research has beenshown to be sensitive to increments in family income, particularlywhen looking at children born into poverty (Totsika &amp; Sylva,2004). The measure includes 55 items, clustered in eight subscales(i.e., learning materials, language stimulation, physical environ-ment, parental responsivity, learning stimulation, modeling of so-cial maturity, variety in experience, and acceptance of child). The first five observations were independently coded by two researchassistants; interrater reliability was_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0005__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003_.95. Once interrater reli-ability was established, a single coder coded subsequent observa-tions.” (p. 106–107)</t>
   </si>
   <si>
     <t xml:space="preserve">Newcomb, Michael D.;Abbott, Robert D.;Catalano, Richard F.;Hawkins, J. David;Battin-Pearson, Sara;Hill, Karl</t>
@@ -3764,7 +3762,7 @@
     <t xml:space="preserve">Emotions and physical health in the second half of life: Interindividual differences in age-related trajectories and dynamic associations according to socioeconomic status</t>
   </si>
   <si>
-    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
+    <t xml:space="preserve">Education was used as an indicator for SES in the present study. Participants reported their highest level of completed school education with reference to the German education scheme. As more than 50% had low education, only two levels of education were distinguished to avoid largely unequal group sizes: low (basic school degree or no degree, corresponding to less than 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 2,405, 62.5% of the sample) and high (middle or advanced school degree, corresponding to at least 10 years of school education; n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 1,442, 37.5% of the sample). (pg.341)</t>
   </si>
   <si>
     <t xml:space="preserve">In the Reserve Capacity Model by Gallo and Matthews (2003), the authors hypothesize that SES is not only linked to physical health but also to the experience of positive and negative emotions. (pg.338)</t>
@@ -3833,12 +3831,12 @@
   </si>
   <si>
     <t xml:space="preserve">"Pilot data within a nationally collected online community
-sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
+sample (n _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ 81), demonstrated this particular measure of social
 class was correlated with household income, a more objective
-measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
+measure of the construct, r _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .51, p  .001. (pg.451)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant’s social class was assessed, as in prior research (Kraus &amp; Keltner, 2009; Lachman &amp; Weaver, 1998), in terms of family income and parental education attainment. Family income was measured in seven categories: (1) below $15,000, (2) $15,001–$25,000, (3) $25,001–$35,000, (4) $35,001– $50,000, (5) $50,001–$75,000, (6) $75,001–$100,000, (7) above $100,000. Median family income for participants in this sample was between $50,001 and $75,000. Parental education was assessed in terms of four categories: (1) less than high school graduation, (2) high school graduation, (3) college degree, (4) postgraduate degree, with the median education attained for both parents as a college degree. Measures of family income and education were intercorrelated, r(64) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .56, p .001. To compute an overall measure of social class we standardized measures of family income and parental education, then computed an average indicating overall social class (e.g., Kraus &amp; Keltner, 2009). The current sample is consistent with other studies of social class, in that 28.8% of parents in our sample, and 31.2% in other nationally collected samples attained high school graduation as their highest level of education completed (Johnson &amp; Krueger, 2005, 2006). The median level income of this sample was also comparable to the 2010 national median income ($51,965) according to the U. S. Census Bureau (DeNavas–Walt, Proctor, &amp; Smith, 2010) (pg. 453).</t>
   </si>
   <si>
     <t xml:space="preserve">In Study 2, social class predicted participants’ compassionrelated subjective reports and autonomic responses associated with
@@ -3861,7 +3859,7 @@
   <si>
     <t xml:space="preserve">Social class was measured in the same manner as
 Study 2. The median family income of the study was between
-$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
+$50,001 and $75,000. Again, measures of family income and education were intercorrelated, r(104) _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0001_ .50 p  .001. To compute an
 overall measure of social class, we standardized measures of family
 income and parental education, and then computed an average indicating overall participant social class (Kraus &amp; Keltner, 2009) (pg. 455).</t>
   </si>
@@ -3901,13 +3899,13 @@
     <t xml:space="preserve">When stress gets into your head: Socioeconomic risk, executive functions, and maternal sensitivity across childrearing contexts</t>
   </si>
   <si>
-    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
+    <t xml:space="preserve">"In order to create an index of socioeconomic risk, we followed previous guidelines (Conger et al., 2010; Dearing, McCartney, &amp; Taylor, 2001) and created a composite variable comprised of a family income-to-needs ratio, maternal education, and maternal report of level of chaos in the neighborhood. Mothers completed a demographics survey in which they reported their level of education, number of people living in the household, and annual household income. Income-to- needs ratio ratings were computed by dividing total family income by poverty-level income based on the number of people living in the home. Poverty income guidelines per persons in household were based upon the 2012 Department of Health and Human Services Poverty Guidelines (U.S. Department of Health and Hu- man Services, 2012, pp. 4034–4035). Income-to-needs ratios be- low 1.00 indicate that the income of the individuals in the home is below the federal definition of poverty. Neighborhood risk was measured using maternal report on the Neighborhood Organization and Affiliation Scale (Knight, Smith, Martin, Lewis, &amp; the LOGSCAN Investigators, 2008). The sub- scale assesses problems in the respondents’ neighborhood (e.g., “There is open drug activity”; “houses are broken into”; “homes get broken into”) on a 4-point scale ranging from strongly disagree to strongly agree. Internal consistency coefficient for the scale washigh (𝛼_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_= .93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood." (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">"It has been demonstrated that higher levels of stress asso- ciated with increased socioeconomic risk (SES)—including crowded housing arrangements, job/financial instability, tense fa- milial relations, sleep deprivation, and poor nutrition/health— have been linked to poorer cognitive regulation of attention and mem- ory, reduced working memory capacity, and diminished emotional regulation capacity in mothers (Crandall et al., 2015; Deater- Deckard, Wang, Chen, &amp; Bell, 2012)." (p. 161)</t>
   </si>
   <si>
-    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
+    <t xml:space="preserve">SA: Great overall! I’d just add to the operationalization: “Internal consistency coefficient for the scale washigh (_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0003__x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_.93). The three risk assessments were significantlycorrelated with one another (rs ranged from .27 to .52) and werestandardized and summed to create a composite measure of socio-economic risk. Higher scores indicated greater risk.” (p. 162). I think the reason should be “In order to create an index ofsocioeconomic risk, we followed previous guidelines (Conger etal., 2010;Dearing, McCartney, &amp; Taylor, 2001) and created acomposite variable comprised of a family income-to-needs ratio,maternal education, and maternal report of level of chaos in theneighborhood.” (p. 162)</t>
   </si>
   <si>
     <t xml:space="preserve">Townsend, Sarah S. M.;Fryberg, Stephanie A.;Wilkins, Clara L.;Markus, Hazel Rose</t>
@@ -3962,14 +3960,15 @@
     <t xml:space="preserve">because many people do not know or are not willing to report their exact absolute income. p.143</t>
   </si>
   <si>
-    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
+    <t xml:space="preserve">As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). </t>
   </si>
   <si>
     <t xml:space="preserve">Pretty good. SES is an IV in this paper (it’s not being predicted). Good job on the theoretical defintion; the only bit I’d add is 
-Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
+Great job on the operationalization for Study 1. For the reason, the quote you have is good; I’d also add the “Like others...” bit. The same sentence could be used for both the operationalization and reason in the case of this paper. Studies 2 and 3 are correct, too, but we need to be pulling the quotes from the studies if there is an appropriate quote within the study. E.g., for Study 2, we would use “As in Study 1, SES was measured with one item target-ing current annual family income, ona1(less than $10,000 peryear)to6($50,000 or above) scale (M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_4.75,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_1.54; seeTable 1).” (p. 145). for study 3, we would use “As in Studies 1 and 2, SES was measured with one itemassessing current annual family income, ona1(less than $10,000per year)to12($200,000 or above) scale;M_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_5.85,SD_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x
+05F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0002_3.20;seeTable 1).” (p. 148). For the reasons, I would copy over the sentence used for Study 1. ⇒ I have made the adjustments, but it seems like having to find the exact quotes within the study will be taking more time but getting the same info, compared to directly using the quote in the introduction. The contents are the same. </t>
   </si>
   <si>
     <t xml:space="preserve">von Keyserlingk, Luise;Becker, Michael;Jansen, Malte;Maaz, Kai</t>
@@ -4022,7 +4021,7 @@
     <t xml:space="preserve">2860 Gerontology</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
+    <t xml:space="preserve">In addition, the study included three self-report measures of socioeconomic status (SES): education (no education 3.4%, high school or trade 31.8%, university education 34.7%), income (less than $17,000 20.9%, 17,000 to 51,000 58.8%, more than $51,000 20.4%), and perceived socioeconomic status (M 6.14, SD 1.80; Adler, Epel, Castellazzo, &amp; Ickovics, 2000). Because the three SES measures were positively correlated (rs .39 to .53, ps _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0004_ .01), we computed a composite score of SES for further analysis by averaging the three standardized measures (M .02, SD .81). (pg.353)</t>
   </si>
   <si>
     <t xml:space="preserve">Varnum, Michael E. W.;Na, Jinkyung;Murata, Asuka;Kitayama, Shinobu</t>
@@ -4091,7 +4090,7 @@
     <t xml:space="preserve">"However, be-cause global health is self-reported, its association with SSS couldbe confounded by psychological third variables that correlate withboth constructs. In the present study we test whether the associa-tion of SSS with self-reported health is independent of a plausibleclass of confounding variables: negative mood... Research has shown a strong relationship between increased economic inequality and elevated mortality rates among the dis- advantaged and points to the contribution of rank to health in- equality (e.g., Kawachi &amp; Kennedy, 1997). To the extent that relative rank is important in this relationship, subjective percep- tions of SES are likely to be powerful predictors of health and well-being... For instance, even after accounting for effects due to objective indicators of SES (e.g., education, income), SSS uniquely predicts self-rated global health (Adler et al., 2000; Franzini &amp; Fernandez-Esquer, 2006; Hyde &amp; Jones, 2007; Ostrove, Adler, Kuppermann, &amp; Washing- ton, 2000), and negative affect (Adler et al., 2000; Ghaed &amp; Gallo, 2007; Gianaros et al., 2007; Operario et al., 2004)." (p. 138); none given for objective indicators</t>
   </si>
   <si>
-    <t xml:space="preserve">“Control  variables:  Social  class  and  health  risk  factors….Demographic con-trols included level of education (8th grade thru post graduatestudy), age (in years), weekly income (in dollars) and work status(1_x005F_x005F_x005F_x005F_x0006_employed).” p. 1998</t>
+    <t xml:space="preserve">“Control  variables:  Social  class  and  health  risk  factors….Demographic con-trols included level of education (8th grade thru post graduatestudy), age (in years), weekly income (in dollars) and work status(1_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x0006_employed).” p. 1998</t>
   </si>
   <si>
     <t xml:space="preserve">Paper reviews method for MSEM. Example involves examining how SES relation to math scored moderated by school size. Paper did not report details of how any data were collected, processed, etc. Codes given reflect the particular example, rather than the overall paper.</t>
@@ -4100,16 +4099,16 @@
     <t xml:space="preserve">“To further explain the covariance structure of the item-effect variables the model offers the possibility to includeexplanatory variables. We included some explanatoryvariables for the item-effect variables in order to illustratethis option. To check whether gender or social economicstatus (SES; measured by highest educational degree of aperson) explains the multidimensionality, we introducedthese variables as dichotomous (gender with 2 levels) orordered categorical (SES indicator with 8 levels) explana-tory variables for the item-effect variables while controllingfor effects on the latent states (see ESM 4 for input file).” (p. 276)</t>
   </si>
   <si>
-    <t xml:space="preserve">SES as IV: “We asked 30 participants (12 female, 18 male;Mage_x005F_x005F_x0002_36.70years,SD_x005F_x005F_x0002_10.72; 21 Caucasian, three African, two East Asian,two Hispanic, one mixed race, one Pacific Islander) from Ama-zon’s Mechanical Turk (MTurk) to list the emotions that rich andpoor people stereotypically feel, respectively, with the order ofthese two questions randomized.” (p. 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“We randomly assigned 150 MTurk Workers (82female, 65 male, 3 other;Mage_x005F_x005F_x0002_37.46 years,SD_x005F_x005F_x0002_12.44; 109Caucasian, 13 African, nine Hispanic, seven East Asian, fivemixed-race, three Native American, two Southeast Asian, twounspecified ethnicity) to categorize the social class of either the 80rich (N_x005F_x005F_x0002_76) or 80 poor targets (N_x005F_x005F_x0002_74) asrichorpoorat theirown pace” (p. 3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“We randomlyassigned 150 MTurk Workers (68 female, 82 male;Mage_x005F_x005F_x0002_36.07years,SD_x005F_x005F_x0002_12.09; 108 Caucasian, 11 African, 10 East Asian, 10Hispanic, five Native American, two mixed race, one MiddleEastern, one South Asian, one Southeast Asian, one unspecifiedethnicity) to categorize the social class of either the 80 rich (N_x005F_x005F_x0002_72) or 80 poor targets (N_x005F_x005F_x0002_78) asrichorpoorin random order.” (p. 4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“We recruited 150 MTurk Workers (50 female,100 male;Mage_x005F_x005F_x0002_35.04 years,SD_x005F_x005F_x0002_11.22; 93 Caucasian, 35African, seven Hispanic, four East Asian, four mixed race, threeNative American, two Southeast Asian, one South Asian, oneunspecified ethnicity) to categorize the targets asrichorpoor.” (p. 5)</t>
+    <t xml:space="preserve">SES as IV: “We asked 30 participants (12 female, 18 male;Mage_x005F_x005F_x005F_x005F_x0002_36.70years,SD_x005F_x005F_x005F_x005F_x0002_10.72; 21 Caucasian, three African, two East Asian,two Hispanic, one mixed race, one Pacific Islander) from Ama-zon’s Mechanical Turk (MTurk) to list the emotions that rich andpoor people stereotypically feel, respectively, with the order ofthese two questions randomized.” (p. 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“We randomly assigned 150 MTurk Workers (82female, 65 male, 3 other;Mage_x005F_x005F_x005F_x005F_x0002_37.46 years,SD_x005F_x005F_x005F_x005F_x0002_12.44; 109Caucasian, 13 African, nine Hispanic, seven East Asian, fivemixed-race, three Native American, two Southeast Asian, twounspecified ethnicity) to categorize the social class of either the 80rich (N_x005F_x005F_x005F_x005F_x0002_76) or 80 poor targets (N_x005F_x005F_x005F_x005F_x0002_74) asrichorpoorat theirown pace” (p. 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“We randomlyassigned 150 MTurk Workers (68 female, 82 male;Mage_x005F_x005F_x005F_x005F_x0002_36.07years,SD_x005F_x005F_x005F_x005F_x0002_12.09; 108 Caucasian, 11 African, 10 East Asian, 10Hispanic, five Native American, two mixed race, one MiddleEastern, one South Asian, one Southeast Asian, one unspecifiedethnicity) to categorize the social class of either the 80 rich (N_x005F_x005F_x005F_x005F_x0002_72) or 80 poor targets (N_x005F_x005F_x005F_x005F_x0002_78) asrichorpoorin random order.” (p. 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“We recruited 150 MTurk Workers (50 female,100 male;Mage_x005F_x005F_x005F_x005F_x0002_35.04 years,SD_x005F_x005F_x005F_x005F_x0002_11.22; 93 Caucasian, 35African, seven Hispanic, four East Asian, four mixed race, threeNative American, two Southeast Asian, one South Asian, oneunspecified ethnicity) to categorize the targets asrichorpoor.” (p. 5)</t>
   </si>
   <si>
     <t xml:space="preserve">“We asked partic-ipants to categorize each face as eitherpoor,working class,middleclass,upper-middle class,orupper class.” (p. 6)</t>
@@ -4118,10 +4117,19 @@
     <t xml:space="preserve">“Although Studies 1 and 2 helped illustrate the strong associationbetween negative emotion and low social class standing, socialclass group membership is more nuanced than justrichversuspoor—these describe only the extremes of the social class spec-trum. People often think of social class categorically, using termssuch aspoor,working class,middle class,upper-middle class, andupper class(Jackman &amp; Jackman, 1983). It therefore remainsunknown whether people use emotional expressions to make morespecific social class judgments, rather than just to evaluate lowversus high class standing….We chose these partic-ular class labels because they are intuitive and understandable toNorth Americans (see Jackman &amp; Jackman, 1983) and becauserecent research has used them effectively (e.g., Dietze &amp; Knowles,2016). “ (p. 6)</t>
   </si>
   <si>
-    <t xml:space="preserve">“Education was coded to be on a5-point interval scale (no schooling/elementary school, some highschool, high school completion, some postsecondary, and anypostsecondary completion) and income was coded to be on a12-point interval scale (no incometo$100 000_x005F_x005F_x0006_).” (p. 337)</t>
+    <t xml:space="preserve">“Education was coded to be on a5-point interval scale (no schooling/elementary school, some highschool, high school completion, some postsecondary, and anypostsecondary completion) and income was coded to be on a12-point interval scale (no incometo$100 000_x005F_x005F_x005F_x005F_x0006_).” (p. 337)</t>
   </si>
   <si>
     <t xml:space="preserve">“One set of factors that may influence the R/R–mastery relation-ship are structural resources, namely things that would broadly fallunder socioeconomic status (e.g., education, income). Higher lev-els of education are associated with higher levels of mastery andfinancial resources promote a sense of power and implicit mobil-ity. Persons with higher levels of education have a greater capacityto attend to problems, to solve problems, and consequently havebetter job stability and security (Ross &amp; Mirowsky, 2013). Finan-cially secure persons are able to leverage their financial stability tobuttress their sense of autonomy. Overall, persons high in educa-tion or income are more likely to perceive themselves as autono-mous, and this autonomy may mitigate the adverse effects ofmastery-inhibiting factors (for example, age;Ross &amp; Mirowsky,2013).Because structural resources have a well-documented relation-ship with mastery (Ross &amp; Mirowsky, 2013), several researchershave investigated whether structural resources may account for theinconsistent relationship between R/R–mastery. But even whenexamining structural resources, there is still disagreement as to therelationship between R/R and mastery. At a basic level, research-ers tend to agree that greater structural resources are associatedwith greater mastery, but will dispute whether R/R willexacerbatedifferences in mastery between a high resource group (i.e., higheducation/high income) and a low resource group (i.e., low edu-cation/low income), or whether R/R willmitigatethe differences inmastery. These two competing viewpoints, which are described asresource amplification and resource compensation respectively,acknowledge that structural resources moderate the relationshipbetween R/R and mastery but differ on the whether this modera-tion is positive or negative (Mirowsky &amp; Ross, 1998;Schieman etal., 2003).” (p. 334)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other composite_two factor Hollingshead index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple single indicators_maternal income-maternal education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single indicator_maternal income [dichotomized]</t>
   </si>
 </sst>
 </file>
@@ -28885,10 +28893,10 @@
   <dimension ref="A1:AH263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E234" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A234" activeCellId="0" sqref="A234"/>
+      <selection pane="bottomLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
       <selection pane="bottomRight" activeCell="E257" activeCellId="0" sqref="E257"/>
     </sheetView>
   </sheetViews>
@@ -41029,11 +41037,11 @@
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E186" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A186" activeCellId="0" sqref="A186"/>
-      <selection pane="bottomRight" activeCell="A218" activeCellId="0" sqref="A218"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="N37" activeCellId="0" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42085,7 +42093,7 @@
         <v>291</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>156</v>
+        <v>1139</v>
       </c>
       <c r="O32" s="0" t="s">
         <v>157</v>
@@ -42135,7 +42143,7 @@
         <v>291</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>166</v>
+        <v>1140</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>167</v>
@@ -42182,7 +42190,7 @@
         <v>291</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>172</v>
+        <v>1141</v>
       </c>
       <c r="O34" s="10" t="s">
         <v>291</v>

</xml_diff>